<commit_message>
the protocol-body length must > 0
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/NPC.xlsx
+++ b/_Out/NFDataCfg/Excel/NPC.xlsx
@@ -1832,8 +1832,8 @@
   <dimension ref="A1:AI62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
removed unused server modified the move message's body
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/NPC.xlsx
+++ b/_Out/NFDataCfg/Excel/NPC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="424">
   <si>
     <t>Id</t>
   </si>
@@ -1299,6 +1299,12 @@
   </si>
   <si>
     <t>DescID_Samurai</t>
+  </si>
+  <si>
+    <t>AIOwnerID</t>
+  </si>
+  <si>
+    <t>AI</t>
   </si>
 </sst>
 </file>
@@ -2033,11 +2039,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ62"/>
+  <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ25" sqref="AJ25"/>
+      <selection pane="bottomLeft" activeCell="AI11" sqref="AI11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2065,11 +2071,11 @@
     <col min="30" max="30" width="22.1328125" customWidth="1"/>
     <col min="31" max="31" width="36" customWidth="1"/>
     <col min="32" max="32" width="9.9296875" customWidth="1"/>
-    <col min="34" max="34" width="12.59765625" customWidth="1"/>
-    <col min="36" max="36" width="25" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="12.59765625" customWidth="1"/>
+    <col min="37" max="37" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="14.25">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="14.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2173,13 +2179,16 @@
         <v>23</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" ht="14.25">
+    <row r="2" spans="1:37" s="2" customFormat="1" ht="14.25">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
@@ -2283,13 +2292,16 @@
         <v>29</v>
       </c>
       <c r="AI2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:36" s="2" customFormat="1" ht="14.25">
+    <row r="3" spans="1:37" s="2" customFormat="1" ht="14.25">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -2393,13 +2405,16 @@
         <v>1</v>
       </c>
       <c r="AI3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36" s="2" customFormat="1" ht="14.25">
+    <row r="4" spans="1:37" s="2" customFormat="1" ht="14.25">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
@@ -2503,13 +2518,16 @@
         <v>1</v>
       </c>
       <c r="AI4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="2" customFormat="1" ht="14.25">
+    <row r="5" spans="1:37" s="2" customFormat="1" ht="14.25">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -2613,13 +2631,16 @@
         <v>1</v>
       </c>
       <c r="AI5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5" s="2">
         <v>0</v>
       </c>
+      <c r="AK5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" s="2" customFormat="1" ht="14.25">
+    <row r="6" spans="1:37" s="2" customFormat="1" ht="14.25">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
@@ -2728,8 +2749,11 @@
       <c r="AJ6" s="2">
         <v>0</v>
       </c>
+      <c r="AK6" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" s="3" customFormat="1">
+    <row r="7" spans="1:37" s="3" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>34</v>
       </c>
@@ -2838,8 +2862,11 @@
       <c r="AJ7" s="3">
         <v>0</v>
       </c>
+      <c r="AK7" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" s="3" customFormat="1">
+    <row r="8" spans="1:37" s="3" customFormat="1">
       <c r="A8" s="7" t="s">
         <v>283</v>
       </c>
@@ -2948,8 +2975,11 @@
       <c r="AJ8" s="3">
         <v>0</v>
       </c>
+      <c r="AK8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" s="3" customFormat="1">
+    <row r="9" spans="1:37" s="3" customFormat="1">
       <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
@@ -3058,8 +3088,11 @@
       <c r="AJ9" s="3">
         <v>0</v>
       </c>
+      <c r="AK9" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" s="4" customFormat="1" ht="40.9" thickBot="1">
+    <row r="10" spans="1:37" s="4" customFormat="1" ht="40.9" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>36</v>
       </c>
@@ -3148,13 +3181,16 @@
         <v>59</v>
       </c>
       <c r="AI10" s="4" t="s">
-        <v>369</v>
+        <v>423</v>
       </c>
       <c r="AJ10" s="4" t="s">
         <v>369</v>
       </c>
+      <c r="AK10" s="4" t="s">
+        <v>369</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" ht="13.9" thickBot="1">
+    <row r="11" spans="1:37" ht="13.9" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>60</v>
       </c>
@@ -3245,11 +3281,14 @@
       <c r="AI11">
         <v>0</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="13.9" thickBot="1">
+    <row r="12" spans="1:37" ht="13.9" thickBot="1">
       <c r="A12" t="s">
         <v>308</v>
       </c>
@@ -3340,11 +3379,14 @@
       <c r="AI12">
         <v>0</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="13.9" thickBot="1">
+    <row r="13" spans="1:37" ht="13.9" thickBot="1">
       <c r="A13" t="s">
         <v>307</v>
       </c>
@@ -3435,11 +3477,14 @@
       <c r="AI13">
         <v>0</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="13.9" thickBot="1">
+    <row r="14" spans="1:37" ht="13.9" thickBot="1">
       <c r="A14" t="s">
         <v>306</v>
       </c>
@@ -3530,11 +3575,14 @@
       <c r="AI14">
         <v>0</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="13.9" thickBot="1">
+    <row r="15" spans="1:37" ht="13.9" thickBot="1">
       <c r="A15" t="s">
         <v>305</v>
       </c>
@@ -3625,11 +3673,14 @@
       <c r="AI15">
         <v>0</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AJ15">
+        <v>0</v>
+      </c>
+      <c r="AK15" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="13.9" thickBot="1">
+    <row r="16" spans="1:37" ht="13.9" thickBot="1">
       <c r="A16" t="s">
         <v>304</v>
       </c>
@@ -3720,11 +3771,14 @@
       <c r="AI16">
         <v>0</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AJ16">
+        <v>0</v>
+      </c>
+      <c r="AK16" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="13.9" thickBot="1">
+    <row r="17" spans="1:37" ht="13.9" thickBot="1">
       <c r="A17" t="s">
         <v>302</v>
       </c>
@@ -3815,11 +3869,14 @@
       <c r="AI17">
         <v>0</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="13.9" thickBot="1">
+    <row r="18" spans="1:37" ht="13.9" thickBot="1">
       <c r="A18" t="s">
         <v>303</v>
       </c>
@@ -3910,11 +3967,14 @@
       <c r="AI18">
         <v>0</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="13.9" thickBot="1">
+    <row r="19" spans="1:37" ht="13.9" thickBot="1">
       <c r="A19" t="s">
         <v>301</v>
       </c>
@@ -4005,11 +4065,14 @@
       <c r="AI19">
         <v>0</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+      <c r="AK19" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="13.9" thickBot="1">
+    <row r="20" spans="1:37" ht="13.9" thickBot="1">
       <c r="A20" t="s">
         <v>300</v>
       </c>
@@ -4100,11 +4163,14 @@
       <c r="AI20">
         <v>0</v>
       </c>
-      <c r="AJ20" t="s">
+      <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="13.9" thickBot="1">
+    <row r="21" spans="1:37" ht="13.9" thickBot="1">
       <c r="A21" t="s">
         <v>299</v>
       </c>
@@ -4195,11 +4261,14 @@
       <c r="AI21">
         <v>0</v>
       </c>
-      <c r="AJ21" t="s">
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="13.9" thickBot="1">
+    <row r="22" spans="1:37" ht="13.9" thickBot="1">
       <c r="A22" t="s">
         <v>298</v>
       </c>
@@ -4290,11 +4359,14 @@
       <c r="AI22">
         <v>0</v>
       </c>
-      <c r="AJ22" s="39" t="s">
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="39" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="23" spans="1:36" s="30" customFormat="1" ht="13.9" thickBot="1">
+    <row r="23" spans="1:37" s="30" customFormat="1" ht="13.9" thickBot="1">
       <c r="A23" s="29" t="s">
         <v>66</v>
       </c>
@@ -4397,11 +4469,14 @@
       <c r="AI23" s="30">
         <v>0</v>
       </c>
-      <c r="AJ23" s="34" t="s">
+      <c r="AJ23" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="34" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="24" spans="1:36" s="27" customFormat="1" ht="13.9" thickBot="1">
+    <row r="24" spans="1:37" s="27" customFormat="1" ht="13.9" thickBot="1">
       <c r="A24" s="34" t="s">
         <v>68</v>
       </c>
@@ -4504,11 +4579,14 @@
       <c r="AI24" s="27">
         <v>0</v>
       </c>
-      <c r="AJ24" s="34" t="s">
+      <c r="AJ24" s="27">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="34" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="25" spans="1:36" s="27" customFormat="1" ht="13.9" thickBot="1">
+    <row r="25" spans="1:37" s="27" customFormat="1" ht="13.9" thickBot="1">
       <c r="A25" s="34" t="s">
         <v>70</v>
       </c>
@@ -4611,11 +4689,14 @@
       <c r="AI25" s="27">
         <v>0</v>
       </c>
-      <c r="AJ25" s="34" t="s">
+      <c r="AJ25" s="27">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="34" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="26" spans="1:36" s="27" customFormat="1">
+    <row r="26" spans="1:37" s="27" customFormat="1">
       <c r="A26" s="34" t="s">
         <v>320</v>
       </c>
@@ -4718,11 +4799,14 @@
       <c r="AI26" s="27">
         <v>0</v>
       </c>
-      <c r="AJ26" s="38" t="s">
+      <c r="AJ26" s="27">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="38" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="27" spans="1:36" s="25" customFormat="1">
+    <row r="27" spans="1:37" s="25" customFormat="1">
       <c r="A27" s="24" t="s">
         <v>151</v>
       </c>
@@ -4813,11 +4897,14 @@
       <c r="AI27" s="25">
         <v>0</v>
       </c>
-      <c r="AJ27" s="19" t="s">
+      <c r="AJ27" s="25">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="19" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="28" spans="1:36" s="16" customFormat="1">
+    <row r="28" spans="1:37" s="16" customFormat="1">
       <c r="A28" s="19" t="s">
         <v>161</v>
       </c>
@@ -4908,11 +4995,14 @@
       <c r="AI28" s="16">
         <v>0</v>
       </c>
-      <c r="AJ28" s="19" t="s">
+      <c r="AJ28" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="19" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="29" spans="1:36" s="16" customFormat="1">
+    <row r="29" spans="1:37" s="16" customFormat="1">
       <c r="A29" s="19" t="s">
         <v>171</v>
       </c>
@@ -5003,11 +5093,14 @@
       <c r="AI29" s="16">
         <v>0</v>
       </c>
-      <c r="AJ29" s="19" t="s">
+      <c r="AJ29" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="19" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:36" s="16" customFormat="1">
+    <row r="30" spans="1:37" s="16" customFormat="1">
       <c r="A30" s="19" t="s">
         <v>152</v>
       </c>
@@ -5098,11 +5191,14 @@
       <c r="AI30" s="16">
         <v>0</v>
       </c>
-      <c r="AJ30" s="19" t="s">
+      <c r="AJ30" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="19" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:36" s="16" customFormat="1">
+    <row r="31" spans="1:37" s="16" customFormat="1">
       <c r="A31" s="19" t="s">
         <v>162</v>
       </c>
@@ -5193,11 +5289,14 @@
       <c r="AI31" s="16">
         <v>0</v>
       </c>
-      <c r="AJ31" s="19" t="s">
+      <c r="AJ31" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="19" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="32" spans="1:36" s="16" customFormat="1">
+    <row r="32" spans="1:37" s="16" customFormat="1">
       <c r="A32" s="19" t="s">
         <v>172</v>
       </c>
@@ -5288,11 +5387,14 @@
       <c r="AI32" s="16">
         <v>0</v>
       </c>
-      <c r="AJ32" s="19" t="s">
+      <c r="AJ32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="19" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="33" spans="1:36" s="16" customFormat="1">
+    <row r="33" spans="1:37" s="16" customFormat="1">
       <c r="A33" s="19" t="s">
         <v>153</v>
       </c>
@@ -5383,11 +5485,14 @@
       <c r="AI33" s="16">
         <v>0</v>
       </c>
-      <c r="AJ33" s="19" t="s">
+      <c r="AJ33" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="19" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="1:36" s="16" customFormat="1">
+    <row r="34" spans="1:37" s="16" customFormat="1">
       <c r="A34" s="19" t="s">
         <v>163</v>
       </c>
@@ -5478,11 +5583,14 @@
       <c r="AI34" s="16">
         <v>0</v>
       </c>
-      <c r="AJ34" s="19" t="s">
+      <c r="AJ34" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="35" spans="1:36" s="16" customFormat="1">
+    <row r="35" spans="1:37" s="16" customFormat="1">
       <c r="A35" s="19" t="s">
         <v>173</v>
       </c>
@@ -5573,11 +5681,14 @@
       <c r="AI35" s="16">
         <v>0</v>
       </c>
-      <c r="AJ35" s="19" t="s">
+      <c r="AJ35" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK35" s="19" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="36" spans="1:36" s="16" customFormat="1">
+    <row r="36" spans="1:37" s="16" customFormat="1">
       <c r="A36" s="19" t="s">
         <v>154</v>
       </c>
@@ -5668,11 +5779,14 @@
       <c r="AI36" s="16">
         <v>0</v>
       </c>
-      <c r="AJ36" s="19" t="s">
+      <c r="AJ36" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="19" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:36" s="16" customFormat="1">
+    <row r="37" spans="1:37" s="16" customFormat="1">
       <c r="A37" s="19" t="s">
         <v>164</v>
       </c>
@@ -5763,11 +5877,14 @@
       <c r="AI37" s="16">
         <v>0</v>
       </c>
-      <c r="AJ37" s="19" t="s">
+      <c r="AJ37" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK37" s="19" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="38" spans="1:36" s="16" customFormat="1">
+    <row r="38" spans="1:37" s="16" customFormat="1">
       <c r="A38" s="19" t="s">
         <v>174</v>
       </c>
@@ -5858,11 +5975,14 @@
       <c r="AI38" s="16">
         <v>0</v>
       </c>
-      <c r="AJ38" s="19" t="s">
+      <c r="AJ38" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK38" s="19" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="39" spans="1:36" s="16" customFormat="1">
+    <row r="39" spans="1:37" s="16" customFormat="1">
       <c r="A39" s="19" t="s">
         <v>286</v>
       </c>
@@ -5953,11 +6073,14 @@
       <c r="AI39" s="16">
         <v>0</v>
       </c>
-      <c r="AJ39" s="19" t="s">
+      <c r="AJ39" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK39" s="19" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="40" spans="1:36" s="16" customFormat="1">
+    <row r="40" spans="1:37" s="16" customFormat="1">
       <c r="A40" s="19" t="s">
         <v>296</v>
       </c>
@@ -6048,11 +6171,14 @@
       <c r="AI40" s="16">
         <v>0</v>
       </c>
-      <c r="AJ40" s="19" t="s">
+      <c r="AJ40" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK40" s="19" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="41" spans="1:36" s="16" customFormat="1">
+    <row r="41" spans="1:37" s="16" customFormat="1">
       <c r="A41" s="19" t="s">
         <v>297</v>
       </c>
@@ -6143,11 +6269,14 @@
       <c r="AI41" s="16">
         <v>0</v>
       </c>
-      <c r="AJ41" s="19" t="s">
+      <c r="AJ41" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK41" s="19" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="42" spans="1:36" s="16" customFormat="1">
+    <row r="42" spans="1:37" s="16" customFormat="1">
       <c r="A42" s="19" t="s">
         <v>155</v>
       </c>
@@ -6238,11 +6367,14 @@
       <c r="AI42" s="16">
         <v>0</v>
       </c>
-      <c r="AJ42" s="19" t="s">
+      <c r="AJ42" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK42" s="19" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="43" spans="1:36" s="16" customFormat="1">
+    <row r="43" spans="1:37" s="16" customFormat="1">
       <c r="A43" s="19" t="s">
         <v>165</v>
       </c>
@@ -6333,11 +6465,14 @@
       <c r="AI43" s="16">
         <v>0</v>
       </c>
-      <c r="AJ43" s="19" t="s">
+      <c r="AJ43" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK43" s="19" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="44" spans="1:36" s="16" customFormat="1">
+    <row r="44" spans="1:37" s="16" customFormat="1">
       <c r="A44" s="19" t="s">
         <v>175</v>
       </c>
@@ -6428,11 +6563,14 @@
       <c r="AI44" s="16">
         <v>0</v>
       </c>
-      <c r="AJ44" s="19" t="s">
+      <c r="AJ44" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK44" s="19" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="45" spans="1:36" s="16" customFormat="1">
+    <row r="45" spans="1:37" s="16" customFormat="1">
       <c r="A45" s="19" t="s">
         <v>156</v>
       </c>
@@ -6523,11 +6661,14 @@
       <c r="AI45" s="16">
         <v>0</v>
       </c>
-      <c r="AJ45" s="19" t="s">
+      <c r="AJ45" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK45" s="19" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="46" spans="1:36" s="16" customFormat="1">
+    <row r="46" spans="1:37" s="16" customFormat="1">
       <c r="A46" s="19" t="s">
         <v>166</v>
       </c>
@@ -6618,11 +6759,14 @@
       <c r="AI46" s="16">
         <v>0</v>
       </c>
-      <c r="AJ46" s="19" t="s">
+      <c r="AJ46" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="19" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="47" spans="1:36" s="16" customFormat="1">
+    <row r="47" spans="1:37" s="16" customFormat="1">
       <c r="A47" s="19" t="s">
         <v>176</v>
       </c>
@@ -6713,11 +6857,14 @@
       <c r="AI47" s="16">
         <v>0</v>
       </c>
-      <c r="AJ47" s="19" t="s">
+      <c r="AJ47" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="19" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="48" spans="1:36" s="16" customFormat="1">
+    <row r="48" spans="1:37" s="16" customFormat="1">
       <c r="A48" s="19" t="s">
         <v>157</v>
       </c>
@@ -6808,11 +6955,14 @@
       <c r="AI48" s="16">
         <v>0</v>
       </c>
-      <c r="AJ48" s="19" t="s">
+      <c r="AJ48" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK48" s="19" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="49" spans="1:36" s="16" customFormat="1">
+    <row r="49" spans="1:37" s="16" customFormat="1">
       <c r="A49" s="19" t="s">
         <v>167</v>
       </c>
@@ -6903,11 +7053,14 @@
       <c r="AI49" s="16">
         <v>0</v>
       </c>
-      <c r="AJ49" s="19" t="s">
+      <c r="AJ49" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK49" s="19" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="50" spans="1:36" s="16" customFormat="1">
+    <row r="50" spans="1:37" s="16" customFormat="1">
       <c r="A50" s="19" t="s">
         <v>177</v>
       </c>
@@ -6998,11 +7151,14 @@
       <c r="AI50" s="16">
         <v>0</v>
       </c>
-      <c r="AJ50" s="19" t="s">
+      <c r="AJ50" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK50" s="19" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="51" spans="1:36" s="16" customFormat="1">
+    <row r="51" spans="1:37" s="16" customFormat="1">
       <c r="A51" s="19" t="s">
         <v>158</v>
       </c>
@@ -7093,11 +7249,14 @@
       <c r="AI51" s="16">
         <v>0</v>
       </c>
-      <c r="AJ51" s="19" t="s">
+      <c r="AJ51" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK51" s="19" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="52" spans="1:36" s="16" customFormat="1">
+    <row r="52" spans="1:37" s="16" customFormat="1">
       <c r="A52" s="19" t="s">
         <v>168</v>
       </c>
@@ -7188,11 +7347,14 @@
       <c r="AI52" s="16">
         <v>0</v>
       </c>
-      <c r="AJ52" s="19" t="s">
+      <c r="AJ52" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK52" s="19" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="53" spans="1:36" s="16" customFormat="1">
+    <row r="53" spans="1:37" s="16" customFormat="1">
       <c r="A53" s="19" t="s">
         <v>178</v>
       </c>
@@ -7283,11 +7445,14 @@
       <c r="AI53" s="16">
         <v>0</v>
       </c>
-      <c r="AJ53" s="19" t="s">
+      <c r="AJ53" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="19" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="54" spans="1:36" s="16" customFormat="1">
+    <row r="54" spans="1:37" s="16" customFormat="1">
       <c r="A54" s="19" t="s">
         <v>159</v>
       </c>
@@ -7378,11 +7543,14 @@
       <c r="AI54" s="16">
         <v>0</v>
       </c>
-      <c r="AJ54" s="19" t="s">
+      <c r="AJ54" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK54" s="19" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="55" spans="1:36" s="16" customFormat="1">
+    <row r="55" spans="1:37" s="16" customFormat="1">
       <c r="A55" s="19" t="s">
         <v>169</v>
       </c>
@@ -7473,11 +7641,14 @@
       <c r="AI55" s="16">
         <v>0</v>
       </c>
-      <c r="AJ55" s="19" t="s">
+      <c r="AJ55" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK55" s="19" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="56" spans="1:36" s="16" customFormat="1">
+    <row r="56" spans="1:37" s="16" customFormat="1">
       <c r="A56" s="19" t="s">
         <v>179</v>
       </c>
@@ -7568,11 +7739,14 @@
       <c r="AI56" s="16">
         <v>0</v>
       </c>
-      <c r="AJ56" s="19" t="s">
+      <c r="AJ56" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK56" s="19" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="57" spans="1:36" s="16" customFormat="1">
+    <row r="57" spans="1:37" s="16" customFormat="1">
       <c r="A57" s="19" t="s">
         <v>160</v>
       </c>
@@ -7663,11 +7837,14 @@
       <c r="AI57" s="16">
         <v>0</v>
       </c>
-      <c r="AJ57" s="19" t="s">
+      <c r="AJ57" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK57" s="19" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="58" spans="1:36" s="16" customFormat="1" ht="13.9" thickBot="1">
+    <row r="58" spans="1:37" s="16" customFormat="1" ht="13.9" thickBot="1">
       <c r="A58" s="19" t="s">
         <v>170</v>
       </c>
@@ -7758,11 +7935,14 @@
       <c r="AI58" s="16">
         <v>0</v>
       </c>
-      <c r="AJ58" s="20" t="s">
+      <c r="AJ58" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK58" s="20" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="59" spans="1:36" s="21" customFormat="1" ht="13.9" thickBot="1">
+    <row r="59" spans="1:37" s="21" customFormat="1" ht="13.9" thickBot="1">
       <c r="A59" s="20" t="s">
         <v>180</v>
       </c>
@@ -7853,11 +8033,14 @@
       <c r="AI59" s="21">
         <v>0</v>
       </c>
-      <c r="AJ59" s="19" t="s">
+      <c r="AJ59" s="21">
+        <v>0</v>
+      </c>
+      <c r="AK59" s="19" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="60" spans="1:36" s="16" customFormat="1">
+    <row r="60" spans="1:37" s="16" customFormat="1">
       <c r="A60" s="19" t="s">
         <v>181</v>
       </c>
@@ -7948,11 +8131,14 @@
       <c r="AI60" s="16">
         <v>0</v>
       </c>
-      <c r="AJ60" s="19" t="s">
+      <c r="AJ60" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK60" s="19" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="61" spans="1:36" s="16" customFormat="1" ht="13.9" thickBot="1">
+    <row r="61" spans="1:37" s="16" customFormat="1" ht="13.9" thickBot="1">
       <c r="A61" s="19" t="s">
         <v>182</v>
       </c>
@@ -8043,11 +8229,14 @@
       <c r="AI61" s="16">
         <v>0</v>
       </c>
-      <c r="AJ61" s="20" t="s">
+      <c r="AJ61" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK61" s="20" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="62" spans="1:36" s="21" customFormat="1" ht="13.9" thickBot="1">
+    <row r="62" spans="1:37" s="21" customFormat="1" ht="13.9" thickBot="1">
       <c r="A62" s="20" t="s">
         <v>183</v>
       </c>
@@ -8138,14 +8327,17 @@
       <c r="AI62" s="21">
         <v>0</v>
       </c>
-      <c r="AJ62" s="21" t="s">
+      <c r="AJ62" s="21">
+        <v>0</v>
+      </c>
+      <c r="AK62" s="21" t="s">
         <v>417</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y8:Z9 AB8:AB9 AC7:AJ9 B7:Q9 T7:X9 AA7:AA9 R8:S9" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y8:Z9 AB8:AB9 R8:S9 B7:Q9 T7:X9 AA7:AA9 AC7:AK9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
removed unused arg in http module
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/NPC.xlsx
+++ b/_Out/NFDataCfg/Excel/NPC.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="425">
   <si>
     <t>Id</t>
   </si>
@@ -1305,6 +1305,9 @@
   </si>
   <si>
     <t>AI</t>
+  </si>
+  <si>
+    <t>UIResources/BuilderSprite</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1554,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1616,9 +1619,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -2041,9 +2041,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI11" sqref="AI11"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC27" sqref="AC27:AC62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3239,10 +3239,10 @@
       <c r="Q11">
         <v>20</v>
       </c>
-      <c r="R11" s="36" t="s">
+      <c r="R11" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="S11" s="36" t="s">
+      <c r="S11" s="35" t="s">
         <v>357</v>
       </c>
       <c r="X11">
@@ -3257,7 +3257,7 @@
       <c r="AA11">
         <v>0</v>
       </c>
-      <c r="AB11" s="37" t="s">
+      <c r="AB11" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC11" s="12" t="s">
@@ -3337,10 +3337,10 @@
       <c r="Q12">
         <v>20</v>
       </c>
-      <c r="R12" s="36" t="s">
+      <c r="R12" s="35" t="s">
         <v>334</v>
       </c>
-      <c r="S12" s="36" t="s">
+      <c r="S12" s="35" t="s">
         <v>359</v>
       </c>
       <c r="X12">
@@ -3355,7 +3355,7 @@
       <c r="AA12">
         <v>0</v>
       </c>
-      <c r="AB12" s="37" t="s">
+      <c r="AB12" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC12" s="12" t="s">
@@ -3435,10 +3435,10 @@
       <c r="Q13">
         <v>20</v>
       </c>
-      <c r="R13" s="36" t="s">
+      <c r="R13" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="S13" s="36" t="s">
+      <c r="S13" s="35" t="s">
         <v>360</v>
       </c>
       <c r="X13">
@@ -3453,7 +3453,7 @@
       <c r="AA13">
         <v>0</v>
       </c>
-      <c r="AB13" s="37" t="s">
+      <c r="AB13" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC13" s="12" t="s">
@@ -3533,10 +3533,10 @@
       <c r="Q14">
         <v>20</v>
       </c>
-      <c r="R14" s="36" t="s">
+      <c r="R14" s="35" t="s">
         <v>336</v>
       </c>
-      <c r="S14" s="36" t="s">
+      <c r="S14" s="35" t="s">
         <v>361</v>
       </c>
       <c r="X14">
@@ -3551,7 +3551,7 @@
       <c r="AA14">
         <v>0</v>
       </c>
-      <c r="AB14" s="37" t="s">
+      <c r="AB14" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC14" s="12" t="s">
@@ -3631,10 +3631,10 @@
       <c r="Q15">
         <v>20</v>
       </c>
-      <c r="R15" s="36" t="s">
+      <c r="R15" s="35" t="s">
         <v>337</v>
       </c>
-      <c r="S15" s="36" t="s">
+      <c r="S15" s="35" t="s">
         <v>362</v>
       </c>
       <c r="X15">
@@ -3649,7 +3649,7 @@
       <c r="AA15">
         <v>0</v>
       </c>
-      <c r="AB15" s="37" t="s">
+      <c r="AB15" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC15" s="12" t="s">
@@ -3729,10 +3729,10 @@
       <c r="Q16">
         <v>20</v>
       </c>
-      <c r="R16" s="36" t="s">
+      <c r="R16" s="35" t="s">
         <v>338</v>
       </c>
-      <c r="S16" s="36" t="s">
+      <c r="S16" s="35" t="s">
         <v>363</v>
       </c>
       <c r="X16">
@@ -3747,7 +3747,7 @@
       <c r="AA16">
         <v>0</v>
       </c>
-      <c r="AB16" s="37" t="s">
+      <c r="AB16" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC16" s="12" t="s">
@@ -3827,10 +3827,10 @@
       <c r="Q17">
         <v>20</v>
       </c>
-      <c r="R17" s="36" t="s">
+      <c r="R17" s="35" t="s">
         <v>339</v>
       </c>
-      <c r="S17" s="36" t="s">
+      <c r="S17" s="35" t="s">
         <v>364</v>
       </c>
       <c r="X17">
@@ -3845,7 +3845,7 @@
       <c r="AA17">
         <v>0</v>
       </c>
-      <c r="AB17" s="37" t="s">
+      <c r="AB17" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC17" s="12" t="s">
@@ -3925,10 +3925,10 @@
       <c r="Q18">
         <v>20</v>
       </c>
-      <c r="R18" s="36" t="s">
+      <c r="R18" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="S18" s="36" t="s">
+      <c r="S18" s="35" t="s">
         <v>365</v>
       </c>
       <c r="X18">
@@ -3943,7 +3943,7 @@
       <c r="AA18">
         <v>0</v>
       </c>
-      <c r="AB18" s="37" t="s">
+      <c r="AB18" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC18" s="12" t="s">
@@ -4023,10 +4023,10 @@
       <c r="Q19">
         <v>20</v>
       </c>
-      <c r="R19" s="36" t="s">
+      <c r="R19" s="35" t="s">
         <v>341</v>
       </c>
-      <c r="S19" s="36" t="s">
+      <c r="S19" s="35" t="s">
         <v>366</v>
       </c>
       <c r="X19">
@@ -4041,7 +4041,7 @@
       <c r="AA19">
         <v>0</v>
       </c>
-      <c r="AB19" s="37" t="s">
+      <c r="AB19" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC19" s="12" t="s">
@@ -4121,10 +4121,10 @@
       <c r="Q20">
         <v>20</v>
       </c>
-      <c r="R20" s="36" t="s">
+      <c r="R20" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="S20" s="36" t="s">
+      <c r="S20" s="35" t="s">
         <v>367</v>
       </c>
       <c r="X20">
@@ -4139,7 +4139,7 @@
       <c r="AA20">
         <v>0</v>
       </c>
-      <c r="AB20" s="37" t="s">
+      <c r="AB20" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC20" s="12" t="s">
@@ -4219,10 +4219,10 @@
       <c r="Q21">
         <v>20</v>
       </c>
-      <c r="R21" s="36" t="s">
+      <c r="R21" s="35" t="s">
         <v>343</v>
       </c>
-      <c r="S21" s="36" t="s">
+      <c r="S21" s="35" t="s">
         <v>368</v>
       </c>
       <c r="X21">
@@ -4237,7 +4237,7 @@
       <c r="AA21">
         <v>0</v>
       </c>
-      <c r="AB21" s="37" t="s">
+      <c r="AB21" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC21" s="12" t="s">
@@ -4317,10 +4317,10 @@
       <c r="Q22">
         <v>20</v>
       </c>
-      <c r="R22" s="36" t="s">
+      <c r="R22" s="35" t="s">
         <v>344</v>
       </c>
-      <c r="S22" s="36" t="s">
+      <c r="S22" s="35" t="s">
         <v>368</v>
       </c>
       <c r="X22">
@@ -4335,7 +4335,7 @@
       <c r="AA22">
         <v>0</v>
       </c>
-      <c r="AB22" s="37" t="s">
+      <c r="AB22" s="36" t="s">
         <v>328</v>
       </c>
       <c r="AC22" s="12" t="s">
@@ -4362,497 +4362,497 @@
       <c r="AJ22">
         <v>0</v>
       </c>
-      <c r="AK22" s="39" t="s">
+      <c r="AK22" s="38" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="23" spans="1:37" s="30" customFormat="1" ht="13.9" thickBot="1">
-      <c r="A23" s="29" t="s">
+    <row r="23" spans="1:37" s="29" customFormat="1" ht="13.9" thickBot="1">
+      <c r="A23" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="30">
-        <v>0</v>
-      </c>
-      <c r="D23" s="30">
+      <c r="C23" s="29">
+        <v>0</v>
+      </c>
+      <c r="D23" s="29">
         <v>100</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="29">
         <v>100</v>
       </c>
-      <c r="F23" s="30">
-        <v>0</v>
-      </c>
-      <c r="G23" s="30">
-        <v>0</v>
-      </c>
-      <c r="H23" s="30">
-        <v>0</v>
-      </c>
-      <c r="I23" s="30">
-        <v>0</v>
-      </c>
-      <c r="J23" s="30">
-        <v>0</v>
-      </c>
-      <c r="K23" s="30">
-        <v>0</v>
-      </c>
-      <c r="L23" s="30">
-        <v>0</v>
-      </c>
-      <c r="M23" s="30">
-        <v>0</v>
-      </c>
-      <c r="N23" s="30">
-        <v>2</v>
-      </c>
-      <c r="O23" s="30" t="s">
+      <c r="F23" s="29">
+        <v>0</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0</v>
+      </c>
+      <c r="H23" s="29">
+        <v>0</v>
+      </c>
+      <c r="I23" s="29">
+        <v>0</v>
+      </c>
+      <c r="J23" s="29">
+        <v>0</v>
+      </c>
+      <c r="K23" s="29">
+        <v>0</v>
+      </c>
+      <c r="L23" s="29">
+        <v>0</v>
+      </c>
+      <c r="M23" s="29">
+        <v>0</v>
+      </c>
+      <c r="N23" s="29">
+        <v>2</v>
+      </c>
+      <c r="O23" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="P23" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="30">
+      <c r="P23" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="29">
         <v>20</v>
       </c>
-      <c r="R23" s="35" t="s">
+      <c r="R23" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="S23" s="35" t="s">
+      <c r="S23" s="34" t="s">
         <v>357</v>
       </c>
-      <c r="T23" s="30" t="s">
+      <c r="T23" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="U23" s="30" t="s">
+      <c r="U23" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="V23" s="30" t="s">
+      <c r="V23" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="W23" s="30" t="s">
+      <c r="W23" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="X23" s="30">
-        <v>2</v>
-      </c>
-      <c r="Y23" s="31" t="s">
+      <c r="X23" s="29">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="Z23" s="30" t="s">
+      <c r="Z23" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="AA23" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="30" t="s">
+      <c r="AA23" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="AC23" s="32" t="s">
+      <c r="AC23" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="AD23" s="33" t="s">
+      <c r="AD23" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="AE23" s="30" t="s">
+      <c r="AE23" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="AF23" s="30">
-        <v>0</v>
-      </c>
-      <c r="AG23" s="30">
-        <v>0</v>
-      </c>
-      <c r="AH23" s="30">
-        <v>0</v>
-      </c>
-      <c r="AI23" s="30">
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="30">
-        <v>0</v>
-      </c>
-      <c r="AK23" s="34" t="s">
+      <c r="AF23" s="29">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="29">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="29">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="29">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="33" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="24" spans="1:37" s="27" customFormat="1" ht="13.9" thickBot="1">
-      <c r="A24" s="34" t="s">
+    <row r="24" spans="1:37" s="26" customFormat="1" ht="13.9" thickBot="1">
+      <c r="A24" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="27">
-        <v>0</v>
-      </c>
-      <c r="D24" s="30">
+      <c r="C24" s="26">
+        <v>0</v>
+      </c>
+      <c r="D24" s="29">
         <v>100</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="29">
         <v>100</v>
       </c>
-      <c r="F24" s="27">
-        <v>0</v>
-      </c>
-      <c r="G24" s="27">
-        <v>0</v>
-      </c>
-      <c r="H24" s="27">
-        <v>0</v>
-      </c>
-      <c r="I24" s="27">
-        <v>0</v>
-      </c>
-      <c r="J24" s="27">
-        <v>0</v>
-      </c>
-      <c r="K24" s="27">
-        <v>0</v>
-      </c>
-      <c r="L24" s="27">
-        <v>0</v>
-      </c>
-      <c r="M24" s="27">
-        <v>0</v>
-      </c>
-      <c r="N24" s="30">
-        <v>2</v>
-      </c>
-      <c r="O24" s="27" t="s">
+      <c r="F24" s="26">
+        <v>0</v>
+      </c>
+      <c r="G24" s="26">
+        <v>0</v>
+      </c>
+      <c r="H24" s="26">
+        <v>0</v>
+      </c>
+      <c r="I24" s="26">
+        <v>0</v>
+      </c>
+      <c r="J24" s="26">
+        <v>0</v>
+      </c>
+      <c r="K24" s="26">
+        <v>0</v>
+      </c>
+      <c r="L24" s="26">
+        <v>0</v>
+      </c>
+      <c r="M24" s="26">
+        <v>0</v>
+      </c>
+      <c r="N24" s="29">
+        <v>2</v>
+      </c>
+      <c r="O24" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="P24" s="27">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="27">
+      <c r="P24" s="26">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="26">
         <v>20</v>
       </c>
-      <c r="R24" s="35" t="s">
+      <c r="R24" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="S24" s="35" t="s">
+      <c r="S24" s="34" t="s">
         <v>359</v>
       </c>
-      <c r="T24" s="27" t="s">
+      <c r="T24" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="U24" s="27" t="s">
+      <c r="U24" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="V24" s="27" t="s">
+      <c r="V24" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="W24" s="27" t="s">
+      <c r="W24" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="X24" s="27">
-        <v>2</v>
-      </c>
-      <c r="Y24" s="31" t="s">
+      <c r="X24" s="26">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="Z24" s="27" t="s">
+      <c r="Z24" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AA24" s="27">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="27" t="s">
+      <c r="AA24" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="AC24" s="28" t="s">
+      <c r="AC24" s="27" t="s">
         <v>327</v>
       </c>
       <c r="AD24" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="AE24" s="27" t="s">
+      <c r="AE24" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="AF24" s="27">
-        <v>0</v>
-      </c>
-      <c r="AG24" s="27">
-        <v>0</v>
-      </c>
-      <c r="AH24" s="27">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="27">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="27">
-        <v>0</v>
-      </c>
-      <c r="AK24" s="34" t="s">
+      <c r="AF24" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="26">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="33" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="25" spans="1:37" s="27" customFormat="1" ht="13.9" thickBot="1">
-      <c r="A25" s="34" t="s">
+    <row r="25" spans="1:37" s="26" customFormat="1" ht="13.9" thickBot="1">
+      <c r="A25" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="27">
-        <v>0</v>
-      </c>
-      <c r="D25" s="30">
+      <c r="C25" s="26">
+        <v>0</v>
+      </c>
+      <c r="D25" s="29">
         <v>100</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="29">
         <v>100</v>
       </c>
-      <c r="F25" s="27">
-        <v>0</v>
-      </c>
-      <c r="G25" s="27">
-        <v>0</v>
-      </c>
-      <c r="H25" s="27">
-        <v>0</v>
-      </c>
-      <c r="I25" s="27">
-        <v>0</v>
-      </c>
-      <c r="J25" s="27">
-        <v>0</v>
-      </c>
-      <c r="K25" s="27">
-        <v>0</v>
-      </c>
-      <c r="L25" s="27">
-        <v>0</v>
-      </c>
-      <c r="M25" s="27">
-        <v>0</v>
-      </c>
-      <c r="N25" s="30">
-        <v>2</v>
-      </c>
-      <c r="O25" s="27" t="s">
+      <c r="F25" s="26">
+        <v>0</v>
+      </c>
+      <c r="G25" s="26">
+        <v>0</v>
+      </c>
+      <c r="H25" s="26">
+        <v>0</v>
+      </c>
+      <c r="I25" s="26">
+        <v>0</v>
+      </c>
+      <c r="J25" s="26">
+        <v>0</v>
+      </c>
+      <c r="K25" s="26">
+        <v>0</v>
+      </c>
+      <c r="L25" s="26">
+        <v>0</v>
+      </c>
+      <c r="M25" s="26">
+        <v>0</v>
+      </c>
+      <c r="N25" s="29">
+        <v>2</v>
+      </c>
+      <c r="O25" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="P25" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="27">
+      <c r="P25" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="26">
         <v>20</v>
       </c>
-      <c r="R25" s="35" t="s">
+      <c r="R25" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="S25" s="35" t="s">
+      <c r="S25" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="T25" s="27" t="s">
+      <c r="T25" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="U25" s="27" t="s">
+      <c r="U25" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="V25" s="27" t="s">
+      <c r="V25" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="W25" s="27" t="s">
+      <c r="W25" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="X25" s="27">
-        <v>2</v>
-      </c>
-      <c r="Y25" s="31" t="s">
+      <c r="X25" s="26">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="Z25" s="27" t="s">
+      <c r="Z25" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AA25" s="27">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="27" t="s">
+      <c r="AA25" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="AC25" s="28" t="s">
+      <c r="AC25" s="27" t="s">
         <v>327</v>
       </c>
       <c r="AD25" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="AE25" s="27" t="s">
+      <c r="AE25" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="AF25" s="27">
-        <v>0</v>
-      </c>
-      <c r="AG25" s="27">
-        <v>0</v>
-      </c>
-      <c r="AH25" s="27">
-        <v>0</v>
-      </c>
-      <c r="AI25" s="27">
-        <v>0</v>
-      </c>
-      <c r="AJ25" s="27">
-        <v>0</v>
-      </c>
-      <c r="AK25" s="34" t="s">
+      <c r="AF25" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="26">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="33" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="26" spans="1:37" s="27" customFormat="1">
-      <c r="A26" s="34" t="s">
+    <row r="26" spans="1:37" s="26" customFormat="1">
+      <c r="A26" s="33" t="s">
         <v>320</v>
       </c>
-      <c r="C26" s="27">
-        <v>0</v>
-      </c>
-      <c r="D26" s="30">
+      <c r="C26" s="26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="29">
         <v>100</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="29">
         <v>100</v>
       </c>
-      <c r="F26" s="27">
-        <v>0</v>
-      </c>
-      <c r="G26" s="27">
-        <v>0</v>
-      </c>
-      <c r="H26" s="27">
-        <v>0</v>
-      </c>
-      <c r="I26" s="27">
-        <v>0</v>
-      </c>
-      <c r="J26" s="27">
-        <v>0</v>
-      </c>
-      <c r="K26" s="27">
-        <v>0</v>
-      </c>
-      <c r="L26" s="27">
-        <v>0</v>
-      </c>
-      <c r="M26" s="27">
-        <v>0</v>
-      </c>
-      <c r="N26" s="30">
-        <v>2</v>
-      </c>
-      <c r="O26" s="27" t="s">
+      <c r="F26" s="26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="26">
+        <v>0</v>
+      </c>
+      <c r="I26" s="26">
+        <v>0</v>
+      </c>
+      <c r="J26" s="26">
+        <v>0</v>
+      </c>
+      <c r="K26" s="26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="26">
+        <v>0</v>
+      </c>
+      <c r="M26" s="26">
+        <v>0</v>
+      </c>
+      <c r="N26" s="29">
+        <v>2</v>
+      </c>
+      <c r="O26" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="P26" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="27">
+      <c r="P26" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="26">
         <v>20</v>
       </c>
-      <c r="R26" s="35" t="s">
+      <c r="R26" s="34" t="s">
         <v>348</v>
       </c>
-      <c r="S26" s="35" t="s">
+      <c r="S26" s="34" t="s">
         <v>361</v>
       </c>
-      <c r="T26" s="27" t="s">
+      <c r="T26" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="U26" s="27" t="s">
+      <c r="U26" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="V26" s="27" t="s">
+      <c r="V26" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="W26" s="27" t="s">
+      <c r="W26" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="X26" s="27">
-        <v>2</v>
-      </c>
-      <c r="Y26" s="31" t="s">
+      <c r="X26" s="26">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="Z26" s="27" t="s">
+      <c r="Z26" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AA26" s="27">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="27" t="s">
+      <c r="AA26" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="26" t="s">
         <v>331</v>
       </c>
-      <c r="AC26" s="28" t="s">
+      <c r="AC26" s="27" t="s">
         <v>327</v>
       </c>
       <c r="AD26" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="AE26" s="27" t="s">
+      <c r="AE26" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="AF26" s="27">
-        <v>0</v>
-      </c>
-      <c r="AG26" s="27">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="27">
-        <v>0</v>
-      </c>
-      <c r="AI26" s="27">
-        <v>0</v>
-      </c>
-      <c r="AJ26" s="27">
-        <v>0</v>
-      </c>
-      <c r="AK26" s="38" t="s">
+      <c r="AF26" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="26">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="37" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="27" spans="1:37" s="25" customFormat="1">
-      <c r="A27" s="24" t="s">
+    <row r="27" spans="1:37" s="24" customFormat="1">
+      <c r="A27" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C27" s="25">
-        <v>0</v>
-      </c>
-      <c r="D27" s="25">
+      <c r="C27" s="24">
+        <v>0</v>
+      </c>
+      <c r="D27" s="24">
         <v>100</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="24">
         <v>100</v>
       </c>
-      <c r="F27" s="25">
-        <v>0</v>
-      </c>
-      <c r="G27" s="25">
-        <v>0</v>
-      </c>
-      <c r="H27" s="25">
-        <v>0</v>
-      </c>
-      <c r="I27" s="25">
-        <v>0</v>
-      </c>
-      <c r="J27" s="25">
-        <v>0</v>
-      </c>
-      <c r="K27" s="25">
-        <v>0</v>
-      </c>
-      <c r="L27" s="25">
-        <v>2</v>
-      </c>
-      <c r="M27" s="25">
-        <v>2</v>
-      </c>
-      <c r="N27" s="25">
-        <v>2</v>
-      </c>
-      <c r="O27" s="25" t="s">
+      <c r="F27" s="24">
+        <v>0</v>
+      </c>
+      <c r="G27" s="24">
+        <v>0</v>
+      </c>
+      <c r="H27" s="24">
+        <v>0</v>
+      </c>
+      <c r="I27" s="24">
+        <v>0</v>
+      </c>
+      <c r="J27" s="24">
+        <v>0</v>
+      </c>
+      <c r="K27" s="24">
+        <v>0</v>
+      </c>
+      <c r="L27" s="24">
+        <v>2</v>
+      </c>
+      <c r="M27" s="24">
+        <v>2</v>
+      </c>
+      <c r="N27" s="24">
+        <v>2</v>
+      </c>
+      <c r="O27" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="P27" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="25">
+      <c r="P27" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="24">
         <v>20</v>
       </c>
       <c r="R27" s="17" t="s">
@@ -4861,43 +4861,43 @@
       <c r="S27" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="X27" s="25">
+      <c r="X27" s="24">
         <v>2</v>
       </c>
       <c r="Y27" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="Z27" s="25" t="s">
+      <c r="Z27" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="AA27" s="25">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="25" t="s">
+      <c r="AA27" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="24" t="s">
         <v>217</v>
       </c>
       <c r="AC27" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD27" s="25" t="s">
+        <v>424</v>
+      </c>
+      <c r="AD27" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="AE27" s="26" t="s">
+      <c r="AE27" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="AF27" s="25">
-        <v>0</v>
-      </c>
-      <c r="AG27" s="25">
-        <v>0</v>
-      </c>
-      <c r="AH27" s="25">
-        <v>0</v>
-      </c>
-      <c r="AI27" s="25">
-        <v>0</v>
-      </c>
-      <c r="AJ27" s="25">
+      <c r="AF27" s="24">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="24">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="24">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="24">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="24">
         <v>0</v>
       </c>
       <c r="AK27" s="19" t="s">
@@ -4911,10 +4911,10 @@
       <c r="C28" s="16">
         <v>0</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="24">
         <v>100</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="24">
         <v>100</v>
       </c>
       <c r="F28" s="16">
@@ -4941,10 +4941,10 @@
       <c r="M28" s="16">
         <v>2</v>
       </c>
-      <c r="N28" s="25">
-        <v>2</v>
-      </c>
-      <c r="O28" s="25" t="s">
+      <c r="N28" s="24">
+        <v>2</v>
+      </c>
+      <c r="O28" s="24" t="s">
         <v>185</v>
       </c>
       <c r="P28" s="16">
@@ -4974,8 +4974,8 @@
       <c r="AB28" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="AC28" s="17" t="s">
-        <v>63</v>
+      <c r="AC28" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD28" s="16" t="s">
         <v>251</v>
@@ -5009,10 +5009,10 @@
       <c r="C29" s="16">
         <v>0</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="24">
         <v>100</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="24">
         <v>100</v>
       </c>
       <c r="F29" s="16">
@@ -5039,10 +5039,10 @@
       <c r="M29" s="16">
         <v>2</v>
       </c>
-      <c r="N29" s="25">
-        <v>2</v>
-      </c>
-      <c r="O29" s="25" t="s">
+      <c r="N29" s="24">
+        <v>2</v>
+      </c>
+      <c r="O29" s="24" t="s">
         <v>186</v>
       </c>
       <c r="P29" s="16">
@@ -5072,8 +5072,8 @@
       <c r="AB29" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="AC29" s="17" t="s">
-        <v>63</v>
+      <c r="AC29" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD29" s="16" t="s">
         <v>252</v>
@@ -5107,10 +5107,10 @@
       <c r="C30" s="16">
         <v>0</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="24">
         <v>100</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="24">
         <v>100</v>
       </c>
       <c r="F30" s="16">
@@ -5137,7 +5137,7 @@
       <c r="M30" s="16">
         <v>2</v>
       </c>
-      <c r="N30" s="25">
+      <c r="N30" s="24">
         <v>2</v>
       </c>
       <c r="O30" s="16" t="s">
@@ -5170,8 +5170,8 @@
       <c r="AB30" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="AC30" s="17" t="s">
-        <v>63</v>
+      <c r="AC30" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD30" s="16" t="s">
         <v>253</v>
@@ -5205,10 +5205,10 @@
       <c r="C31" s="16">
         <v>0</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="24">
         <v>100</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="24">
         <v>100</v>
       </c>
       <c r="F31" s="16">
@@ -5235,7 +5235,7 @@
       <c r="M31" s="16">
         <v>2</v>
       </c>
-      <c r="N31" s="25">
+      <c r="N31" s="24">
         <v>2</v>
       </c>
       <c r="O31" s="16" t="s">
@@ -5268,8 +5268,8 @@
       <c r="AB31" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="AC31" s="17" t="s">
-        <v>63</v>
+      <c r="AC31" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD31" s="16" t="s">
         <v>254</v>
@@ -5303,10 +5303,10 @@
       <c r="C32" s="16">
         <v>0</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="24">
         <v>100</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="24">
         <v>100</v>
       </c>
       <c r="F32" s="16">
@@ -5333,7 +5333,7 @@
       <c r="M32" s="16">
         <v>2</v>
       </c>
-      <c r="N32" s="25">
+      <c r="N32" s="24">
         <v>2</v>
       </c>
       <c r="O32" s="16" t="s">
@@ -5366,8 +5366,8 @@
       <c r="AB32" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="AC32" s="17" t="s">
-        <v>63</v>
+      <c r="AC32" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD32" s="16" t="s">
         <v>255</v>
@@ -5401,10 +5401,10 @@
       <c r="C33" s="16">
         <v>0</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="24">
         <v>100</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="24">
         <v>100</v>
       </c>
       <c r="F33" s="16">
@@ -5431,7 +5431,7 @@
       <c r="M33" s="16">
         <v>1</v>
       </c>
-      <c r="N33" s="25">
+      <c r="N33" s="24">
         <v>2</v>
       </c>
       <c r="O33" s="16" t="s">
@@ -5464,8 +5464,8 @@
       <c r="AB33" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="AC33" s="17" t="s">
-        <v>63</v>
+      <c r="AC33" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD33" s="16" t="s">
         <v>256</v>
@@ -5499,10 +5499,10 @@
       <c r="C34" s="16">
         <v>0</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="24">
         <v>100</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="24">
         <v>100</v>
       </c>
       <c r="F34" s="16">
@@ -5529,7 +5529,7 @@
       <c r="M34" s="16">
         <v>1</v>
       </c>
-      <c r="N34" s="25">
+      <c r="N34" s="24">
         <v>2</v>
       </c>
       <c r="O34" s="16" t="s">
@@ -5562,8 +5562,8 @@
       <c r="AB34" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="AC34" s="17" t="s">
-        <v>63</v>
+      <c r="AC34" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD34" s="16" t="s">
         <v>257</v>
@@ -5597,10 +5597,10 @@
       <c r="C35" s="16">
         <v>0</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="24">
         <v>100</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="24">
         <v>100</v>
       </c>
       <c r="F35" s="16">
@@ -5627,7 +5627,7 @@
       <c r="M35" s="16">
         <v>1</v>
       </c>
-      <c r="N35" s="25">
+      <c r="N35" s="24">
         <v>2</v>
       </c>
       <c r="O35" s="16" t="s">
@@ -5660,8 +5660,8 @@
       <c r="AB35" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="AC35" s="17" t="s">
-        <v>63</v>
+      <c r="AC35" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD35" s="16" t="s">
         <v>258</v>
@@ -5695,10 +5695,10 @@
       <c r="C36" s="16">
         <v>0</v>
       </c>
-      <c r="D36" s="25">
+      <c r="D36" s="24">
         <v>100</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="24">
         <v>100</v>
       </c>
       <c r="F36" s="16">
@@ -5725,7 +5725,7 @@
       <c r="M36" s="16">
         <v>3</v>
       </c>
-      <c r="N36" s="25">
+      <c r="N36" s="24">
         <v>3</v>
       </c>
       <c r="O36" s="16" t="s">
@@ -5758,8 +5758,8 @@
       <c r="AB36" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="AC36" s="17" t="s">
-        <v>63</v>
+      <c r="AC36" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD36" s="16" t="s">
         <v>259</v>
@@ -5793,10 +5793,10 @@
       <c r="C37" s="16">
         <v>0</v>
       </c>
-      <c r="D37" s="25">
+      <c r="D37" s="24">
         <v>100</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="24">
         <v>100</v>
       </c>
       <c r="F37" s="16">
@@ -5823,7 +5823,7 @@
       <c r="M37" s="16">
         <v>3</v>
       </c>
-      <c r="N37" s="25">
+      <c r="N37" s="24">
         <v>3</v>
       </c>
       <c r="O37" s="16" t="s">
@@ -5856,8 +5856,8 @@
       <c r="AB37" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="AC37" s="17" t="s">
-        <v>63</v>
+      <c r="AC37" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD37" s="16" t="s">
         <v>260</v>
@@ -5891,10 +5891,10 @@
       <c r="C38" s="16">
         <v>0</v>
       </c>
-      <c r="D38" s="25">
+      <c r="D38" s="24">
         <v>100</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="24">
         <v>100</v>
       </c>
       <c r="F38" s="16">
@@ -5921,7 +5921,7 @@
       <c r="M38" s="16">
         <v>3</v>
       </c>
-      <c r="N38" s="25">
+      <c r="N38" s="24">
         <v>3</v>
       </c>
       <c r="O38" s="16" t="s">
@@ -5954,8 +5954,8 @@
       <c r="AB38" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="AC38" s="17" t="s">
-        <v>63</v>
+      <c r="AC38" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD38" s="16" t="s">
         <v>261</v>
@@ -5989,10 +5989,10 @@
       <c r="C39" s="16">
         <v>0</v>
       </c>
-      <c r="D39" s="25">
+      <c r="D39" s="24">
         <v>100</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E39" s="24">
         <v>100</v>
       </c>
       <c r="F39" s="16">
@@ -6019,7 +6019,7 @@
       <c r="M39" s="16">
         <v>1</v>
       </c>
-      <c r="N39" s="25">
+      <c r="N39" s="24">
         <v>1</v>
       </c>
       <c r="O39" s="16" t="s">
@@ -6052,8 +6052,8 @@
       <c r="AB39" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="AC39" s="17" t="s">
-        <v>63</v>
+      <c r="AC39" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD39" s="16" t="s">
         <v>293</v>
@@ -6087,10 +6087,10 @@
       <c r="C40" s="16">
         <v>0</v>
       </c>
-      <c r="D40" s="25">
+      <c r="D40" s="24">
         <v>100</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E40" s="24">
         <v>100</v>
       </c>
       <c r="F40" s="16">
@@ -6117,7 +6117,7 @@
       <c r="M40" s="16">
         <v>1</v>
       </c>
-      <c r="N40" s="25">
+      <c r="N40" s="24">
         <v>1</v>
       </c>
       <c r="O40" s="16" t="s">
@@ -6150,8 +6150,8 @@
       <c r="AB40" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="AC40" s="17" t="s">
-        <v>63</v>
+      <c r="AC40" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD40" s="16" t="s">
         <v>292</v>
@@ -6185,10 +6185,10 @@
       <c r="C41" s="16">
         <v>0</v>
       </c>
-      <c r="D41" s="25">
+      <c r="D41" s="24">
         <v>100</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="24">
         <v>100</v>
       </c>
       <c r="F41" s="16">
@@ -6215,7 +6215,7 @@
       <c r="M41" s="16">
         <v>1</v>
       </c>
-      <c r="N41" s="25">
+      <c r="N41" s="24">
         <v>1</v>
       </c>
       <c r="O41" s="16" t="s">
@@ -6248,8 +6248,8 @@
       <c r="AB41" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="AC41" s="17" t="s">
-        <v>63</v>
+      <c r="AC41" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD41" s="16" t="s">
         <v>291</v>
@@ -6283,10 +6283,10 @@
       <c r="C42" s="16">
         <v>0</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D42" s="24">
         <v>100</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="24">
         <v>100</v>
       </c>
       <c r="F42" s="16">
@@ -6313,7 +6313,7 @@
       <c r="M42" s="16">
         <v>2</v>
       </c>
-      <c r="N42" s="25">
+      <c r="N42" s="24">
         <v>2</v>
       </c>
       <c r="O42" s="16" t="s">
@@ -6346,8 +6346,8 @@
       <c r="AB42" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="AC42" s="17" t="s">
-        <v>63</v>
+      <c r="AC42" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD42" s="16" t="s">
         <v>262</v>
@@ -6381,10 +6381,10 @@
       <c r="C43" s="16">
         <v>0</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="24">
         <v>100</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="24">
         <v>100</v>
       </c>
       <c r="F43" s="16">
@@ -6411,7 +6411,7 @@
       <c r="M43" s="16">
         <v>2</v>
       </c>
-      <c r="N43" s="25">
+      <c r="N43" s="24">
         <v>2</v>
       </c>
       <c r="O43" s="16" t="s">
@@ -6444,8 +6444,8 @@
       <c r="AB43" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="AC43" s="17" t="s">
-        <v>63</v>
+      <c r="AC43" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD43" s="16" t="s">
         <v>263</v>
@@ -6479,10 +6479,10 @@
       <c r="C44" s="16">
         <v>0</v>
       </c>
-      <c r="D44" s="25">
+      <c r="D44" s="24">
         <v>100</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="24">
         <v>100</v>
       </c>
       <c r="F44" s="16">
@@ -6509,7 +6509,7 @@
       <c r="M44" s="16">
         <v>2</v>
       </c>
-      <c r="N44" s="25">
+      <c r="N44" s="24">
         <v>2</v>
       </c>
       <c r="O44" s="16" t="s">
@@ -6542,8 +6542,8 @@
       <c r="AB44" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="AC44" s="17" t="s">
-        <v>63</v>
+      <c r="AC44" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD44" s="16" t="s">
         <v>264</v>
@@ -6577,10 +6577,10 @@
       <c r="C45" s="16">
         <v>0</v>
       </c>
-      <c r="D45" s="25">
+      <c r="D45" s="24">
         <v>100</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="24">
         <v>100</v>
       </c>
       <c r="F45" s="16">
@@ -6607,7 +6607,7 @@
       <c r="M45" s="16">
         <v>2</v>
       </c>
-      <c r="N45" s="25">
+      <c r="N45" s="24">
         <v>2</v>
       </c>
       <c r="O45" s="16" t="s">
@@ -6640,8 +6640,8 @@
       <c r="AB45" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="AC45" s="17" t="s">
-        <v>63</v>
+      <c r="AC45" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD45" s="16" t="s">
         <v>265</v>
@@ -6675,10 +6675,10 @@
       <c r="C46" s="16">
         <v>0</v>
       </c>
-      <c r="D46" s="25">
+      <c r="D46" s="24">
         <v>100</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="24">
         <v>100</v>
       </c>
       <c r="F46" s="16">
@@ -6705,7 +6705,7 @@
       <c r="M46" s="16">
         <v>2</v>
       </c>
-      <c r="N46" s="25">
+      <c r="N46" s="24">
         <v>2</v>
       </c>
       <c r="O46" s="16" t="s">
@@ -6738,8 +6738,8 @@
       <c r="AB46" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="AC46" s="17" t="s">
-        <v>63</v>
+      <c r="AC46" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD46" s="16" t="s">
         <v>266</v>
@@ -6773,10 +6773,10 @@
       <c r="C47" s="16">
         <v>0</v>
       </c>
-      <c r="D47" s="25">
+      <c r="D47" s="24">
         <v>100</v>
       </c>
-      <c r="E47" s="25">
+      <c r="E47" s="24">
         <v>100</v>
       </c>
       <c r="F47" s="16">
@@ -6803,7 +6803,7 @@
       <c r="M47" s="16">
         <v>2</v>
       </c>
-      <c r="N47" s="25">
+      <c r="N47" s="24">
         <v>2</v>
       </c>
       <c r="O47" s="16" t="s">
@@ -6836,8 +6836,8 @@
       <c r="AB47" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="AC47" s="17" t="s">
-        <v>63</v>
+      <c r="AC47" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD47" s="16" t="s">
         <v>267</v>
@@ -6871,10 +6871,10 @@
       <c r="C48" s="16">
         <v>0</v>
       </c>
-      <c r="D48" s="25">
+      <c r="D48" s="24">
         <v>100</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E48" s="24">
         <v>100</v>
       </c>
       <c r="F48" s="16">
@@ -6901,7 +6901,7 @@
       <c r="M48" s="16">
         <v>3</v>
       </c>
-      <c r="N48" s="25">
+      <c r="N48" s="24">
         <v>3</v>
       </c>
       <c r="O48" s="16" t="s">
@@ -6934,8 +6934,8 @@
       <c r="AB48" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="AC48" s="17" t="s">
-        <v>63</v>
+      <c r="AC48" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD48" s="16" t="s">
         <v>268</v>
@@ -6969,10 +6969,10 @@
       <c r="C49" s="16">
         <v>0</v>
       </c>
-      <c r="D49" s="25">
+      <c r="D49" s="24">
         <v>100</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E49" s="24">
         <v>100</v>
       </c>
       <c r="F49" s="16">
@@ -6999,7 +6999,7 @@
       <c r="M49" s="16">
         <v>3</v>
       </c>
-      <c r="N49" s="25">
+      <c r="N49" s="24">
         <v>3</v>
       </c>
       <c r="O49" s="16" t="s">
@@ -7032,8 +7032,8 @@
       <c r="AB49" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="AC49" s="17" t="s">
-        <v>63</v>
+      <c r="AC49" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD49" s="16" t="s">
         <v>269</v>
@@ -7067,10 +7067,10 @@
       <c r="C50" s="16">
         <v>0</v>
       </c>
-      <c r="D50" s="25">
+      <c r="D50" s="24">
         <v>100</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="24">
         <v>100</v>
       </c>
       <c r="F50" s="16">
@@ -7097,7 +7097,7 @@
       <c r="M50" s="16">
         <v>3</v>
       </c>
-      <c r="N50" s="25">
+      <c r="N50" s="24">
         <v>3</v>
       </c>
       <c r="O50" s="16" t="s">
@@ -7130,8 +7130,8 @@
       <c r="AB50" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="AC50" s="17" t="s">
-        <v>63</v>
+      <c r="AC50" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD50" s="16" t="s">
         <v>270</v>
@@ -7165,10 +7165,10 @@
       <c r="C51" s="16">
         <v>0</v>
       </c>
-      <c r="D51" s="25">
+      <c r="D51" s="24">
         <v>100</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="24">
         <v>100</v>
       </c>
       <c r="F51" s="16">
@@ -7195,7 +7195,7 @@
       <c r="M51" s="16">
         <v>2</v>
       </c>
-      <c r="N51" s="25">
+      <c r="N51" s="24">
         <v>2</v>
       </c>
       <c r="O51" s="16" t="s">
@@ -7228,8 +7228,8 @@
       <c r="AB51" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="AC51" s="17" t="s">
-        <v>63</v>
+      <c r="AC51" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD51" s="16" t="s">
         <v>271</v>
@@ -7263,10 +7263,10 @@
       <c r="C52" s="16">
         <v>0</v>
       </c>
-      <c r="D52" s="25">
+      <c r="D52" s="24">
         <v>100</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="24">
         <v>100</v>
       </c>
       <c r="F52" s="16">
@@ -7293,7 +7293,7 @@
       <c r="M52" s="16">
         <v>2</v>
       </c>
-      <c r="N52" s="25">
+      <c r="N52" s="24">
         <v>2</v>
       </c>
       <c r="O52" s="16" t="s">
@@ -7326,8 +7326,8 @@
       <c r="AB52" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="AC52" s="17" t="s">
-        <v>63</v>
+      <c r="AC52" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD52" s="16" t="s">
         <v>272</v>
@@ -7361,10 +7361,10 @@
       <c r="C53" s="16">
         <v>0</v>
       </c>
-      <c r="D53" s="25">
+      <c r="D53" s="24">
         <v>100</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="24">
         <v>100</v>
       </c>
       <c r="F53" s="16">
@@ -7391,7 +7391,7 @@
       <c r="M53" s="16">
         <v>2</v>
       </c>
-      <c r="N53" s="25">
+      <c r="N53" s="24">
         <v>2</v>
       </c>
       <c r="O53" s="16" t="s">
@@ -7424,8 +7424,8 @@
       <c r="AB53" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="AC53" s="17" t="s">
-        <v>63</v>
+      <c r="AC53" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD53" s="16" t="s">
         <v>273</v>
@@ -7459,10 +7459,10 @@
       <c r="C54" s="16">
         <v>0</v>
       </c>
-      <c r="D54" s="25">
+      <c r="D54" s="24">
         <v>100</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E54" s="24">
         <v>100</v>
       </c>
       <c r="F54" s="16">
@@ -7489,7 +7489,7 @@
       <c r="M54" s="16">
         <v>2</v>
       </c>
-      <c r="N54" s="25">
+      <c r="N54" s="24">
         <v>3</v>
       </c>
       <c r="O54" s="16" t="s">
@@ -7522,8 +7522,8 @@
       <c r="AB54" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="AC54" s="17" t="s">
-        <v>63</v>
+      <c r="AC54" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD54" s="16" t="s">
         <v>274</v>
@@ -7557,10 +7557,10 @@
       <c r="C55" s="16">
         <v>0</v>
       </c>
-      <c r="D55" s="25">
+      <c r="D55" s="24">
         <v>100</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="24">
         <v>100</v>
       </c>
       <c r="F55" s="16">
@@ -7587,7 +7587,7 @@
       <c r="M55" s="16">
         <v>2</v>
       </c>
-      <c r="N55" s="25">
+      <c r="N55" s="24">
         <v>3</v>
       </c>
       <c r="O55" s="16" t="s">
@@ -7620,8 +7620,8 @@
       <c r="AB55" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="AC55" s="17" t="s">
-        <v>63</v>
+      <c r="AC55" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD55" s="16" t="s">
         <v>275</v>
@@ -7655,10 +7655,10 @@
       <c r="C56" s="16">
         <v>0</v>
       </c>
-      <c r="D56" s="25">
+      <c r="D56" s="24">
         <v>100</v>
       </c>
-      <c r="E56" s="25">
+      <c r="E56" s="24">
         <v>100</v>
       </c>
       <c r="F56" s="16">
@@ -7685,7 +7685,7 @@
       <c r="M56" s="16">
         <v>2</v>
       </c>
-      <c r="N56" s="25">
+      <c r="N56" s="24">
         <v>3</v>
       </c>
       <c r="O56" s="16" t="s">
@@ -7718,8 +7718,8 @@
       <c r="AB56" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="AC56" s="17" t="s">
-        <v>63</v>
+      <c r="AC56" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD56" s="16" t="s">
         <v>276</v>
@@ -7753,10 +7753,10 @@
       <c r="C57" s="16">
         <v>0</v>
       </c>
-      <c r="D57" s="25">
+      <c r="D57" s="24">
         <v>100</v>
       </c>
-      <c r="E57" s="25">
+      <c r="E57" s="24">
         <v>100</v>
       </c>
       <c r="F57" s="16">
@@ -7780,10 +7780,10 @@
       <c r="L57" s="16">
         <v>0</v>
       </c>
-      <c r="M57" s="25">
-        <v>2</v>
-      </c>
-      <c r="N57" s="25">
+      <c r="M57" s="24">
+        <v>2</v>
+      </c>
+      <c r="N57" s="24">
         <v>2</v>
       </c>
       <c r="O57" s="16" t="s">
@@ -7816,8 +7816,8 @@
       <c r="AB57" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="AC57" s="17" t="s">
-        <v>63</v>
+      <c r="AC57" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD57" s="16" t="s">
         <v>277</v>
@@ -7851,10 +7851,10 @@
       <c r="C58" s="16">
         <v>0</v>
       </c>
-      <c r="D58" s="25">
+      <c r="D58" s="24">
         <v>100</v>
       </c>
-      <c r="E58" s="25">
+      <c r="E58" s="24">
         <v>100</v>
       </c>
       <c r="F58" s="16">
@@ -7878,10 +7878,10 @@
       <c r="L58" s="16">
         <v>0</v>
       </c>
-      <c r="M58" s="25">
-        <v>2</v>
-      </c>
-      <c r="N58" s="25">
+      <c r="M58" s="24">
+        <v>2</v>
+      </c>
+      <c r="N58" s="24">
         <v>2</v>
       </c>
       <c r="O58" s="16" t="s">
@@ -7914,8 +7914,8 @@
       <c r="AB58" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="AC58" s="17" t="s">
-        <v>63</v>
+      <c r="AC58" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD58" s="16" t="s">
         <v>278</v>
@@ -7949,10 +7949,10 @@
       <c r="C59" s="21">
         <v>0</v>
       </c>
-      <c r="D59" s="25">
+      <c r="D59" s="24">
         <v>100</v>
       </c>
-      <c r="E59" s="25">
+      <c r="E59" s="24">
         <v>100</v>
       </c>
       <c r="F59" s="21">
@@ -7976,10 +7976,10 @@
       <c r="L59" s="21">
         <v>0</v>
       </c>
-      <c r="M59" s="25">
-        <v>2</v>
-      </c>
-      <c r="N59" s="25">
+      <c r="M59" s="24">
+        <v>2</v>
+      </c>
+      <c r="N59" s="24">
         <v>2</v>
       </c>
       <c r="O59" s="16" t="s">
@@ -8012,13 +8012,13 @@
       <c r="AB59" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="AC59" s="22" t="s">
-        <v>63</v>
+      <c r="AC59" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD59" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="AE59" s="23" t="s">
+      <c r="AE59" s="22" t="s">
         <v>64</v>
       </c>
       <c r="AF59" s="21">
@@ -8047,10 +8047,10 @@
       <c r="C60" s="16">
         <v>0</v>
       </c>
-      <c r="D60" s="25">
+      <c r="D60" s="24">
         <v>100</v>
       </c>
-      <c r="E60" s="25">
+      <c r="E60" s="24">
         <v>100</v>
       </c>
       <c r="F60" s="16">
@@ -8077,7 +8077,7 @@
       <c r="M60" s="16">
         <v>1</v>
       </c>
-      <c r="N60" s="25">
+      <c r="N60" s="24">
         <v>2</v>
       </c>
       <c r="O60" s="16" t="s">
@@ -8110,8 +8110,8 @@
       <c r="AB60" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="AC60" s="17" t="s">
-        <v>63</v>
+      <c r="AC60" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD60" s="16" t="s">
         <v>280</v>
@@ -8145,10 +8145,10 @@
       <c r="C61" s="16">
         <v>0</v>
       </c>
-      <c r="D61" s="25">
+      <c r="D61" s="24">
         <v>100</v>
       </c>
-      <c r="E61" s="25">
+      <c r="E61" s="24">
         <v>100</v>
       </c>
       <c r="F61" s="16">
@@ -8175,7 +8175,7 @@
       <c r="M61" s="16">
         <v>1</v>
       </c>
-      <c r="N61" s="25">
+      <c r="N61" s="24">
         <v>2</v>
       </c>
       <c r="O61" s="16" t="s">
@@ -8208,8 +8208,8 @@
       <c r="AB61" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="AC61" s="17" t="s">
-        <v>63</v>
+      <c r="AC61" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD61" s="16" t="s">
         <v>281</v>
@@ -8243,10 +8243,10 @@
       <c r="C62" s="21">
         <v>0</v>
       </c>
-      <c r="D62" s="25">
+      <c r="D62" s="24">
         <v>100</v>
       </c>
-      <c r="E62" s="25">
+      <c r="E62" s="24">
         <v>100</v>
       </c>
       <c r="F62" s="21">
@@ -8273,7 +8273,7 @@
       <c r="M62" s="21">
         <v>1</v>
       </c>
-      <c r="N62" s="25">
+      <c r="N62" s="24">
         <v>2</v>
       </c>
       <c r="O62" s="16" t="s">
@@ -8306,13 +8306,13 @@
       <c r="AB62" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="AC62" s="22" t="s">
-        <v>63</v>
+      <c r="AC62" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="AD62" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="AE62" s="23" t="s">
+      <c r="AE62" s="22" t="s">
         <v>64</v>
       </c>
       <c r="AF62" s="21">

</xml_diff>

<commit_message>
bc maxhp for npc
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/NPC.xlsx
+++ b/_Out/NFDataCfg/Excel/NPC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="9930" activeTab="1"/>
+    <workbookView windowWidth="21495" windowHeight="9930"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -1382,10 +1382,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1427,11 +1427,77 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1443,16 +1509,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1461,6 +1535,28 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1475,104 +1571,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1635,7 +1635,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1647,19 +1761,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1671,139 +1803,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1981,11 +1981,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2005,17 +2031,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2049,38 +2069,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2092,130 +2092,130 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2778,10 +2778,10 @@
   <sheetPr/>
   <dimension ref="A1:AJ62"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AC16" sqref="AC16"/>
+      <selection pane="bottomLeft" activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3075,7 +3075,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="6">
         <v>0</v>
@@ -3108,25 +3108,25 @@
         <v>0</v>
       </c>
       <c r="Z3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB3" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE3" s="6">
         <v>1</v>
       </c>
       <c r="AF3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3" s="6">
         <v>1</v>
@@ -3138,7 +3138,7 @@
         <v>1</v>
       </c>
       <c r="AJ3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" s="6" customFormat="1" ht="15" spans="1:36">
@@ -3146,7 +3146,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -3173,64 +3173,64 @@
         <v>1</v>
       </c>
       <c r="K4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE4" s="6">
         <v>1</v>
@@ -3248,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="AJ4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" s="6" customFormat="1" ht="15" spans="1:36">
@@ -9146,8 +9146,8 @@
   <sheetPr/>
   <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:AF10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -9364,8 +9364,8 @@
       <c r="D3" s="7">
         <v>0</v>
       </c>
-      <c r="E3" s="7">
-        <v>0</v>
+      <c r="E3" s="6">
+        <v>1</v>
       </c>
       <c r="F3" s="7">
         <v>0</v>
@@ -10086,8 +10086,6 @@
       <c r="P10" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
       <c r="S10" s="8" t="s">
         <v>431</v>
       </c>
@@ -10193,7 +10191,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:Q3 R3 S3:V3 W3 X3 Y3:AF3 R7:R9 W7:W9 X7:X9 B7:Q9 S7:V9 Y7:AF9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:D3 F3:Q3 R3 S3:V3 W3 X3 Y3:AF3 R7:R9 W7:W9 X7:X9 B7:Q9 S7:V9 Y7:AF9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>

</xml_diff>

<commit_message>
fixed bugs when the monster using skills
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/NPC.xlsx
+++ b/_Out/NFDataCfg/Excel/NPC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="9930" activeTab="1"/>
+    <workbookView windowWidth="21495" windowHeight="9930"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451">
   <si>
     <t>Id</t>
   </si>
@@ -420,6 +420,9 @@
     <t>SKILL_Magma_Demon_THUMP</t>
   </si>
   <si>
+    <t>NPC_MagmaDemon-Orange</t>
+  </si>
+  <si>
     <t>DescID_Magma Demon-Orange</t>
   </si>
   <si>
@@ -433,6 +436,9 @@
   </si>
   <si>
     <t>97</t>
+  </si>
+  <si>
+    <t>NPC_MagmaDemon-Blue</t>
   </si>
   <si>
     <t>DescID_Magma Demon-Blue</t>
@@ -1427,113 +1433,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1549,7 +1451,119 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1563,16 +1577,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1635,7 +1641,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1653,13 +1755,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1671,31 +1779,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1707,103 +1809,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1972,15 +1978,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2000,7 +1997,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2031,17 +2028,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2065,7 +2056,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2074,148 +2080,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2778,10 +2784,10 @@
   <sheetPr/>
   <dimension ref="A1:AJ62"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AH9" sqref="AH9"/>
+      <selection pane="bottomLeft" activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4530,7 +4536,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" ht="14.25" spans="1:36">
+    <row r="17" spans="1:36">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -4613,7 +4619,7 @@
         <v>81</v>
       </c>
       <c r="AC17" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="AD17" s="39" t="s">
         <v>82</v>
@@ -4634,12 +4640,12 @@
         <v>0</v>
       </c>
       <c r="AJ17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" spans="1:36">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -4678,7 +4684,7 @@
         <v>2</v>
       </c>
       <c r="O18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -4687,10 +4693,10 @@
         <v>20</v>
       </c>
       <c r="R18" s="25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="S18" s="25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="T18" s="29" t="s">
         <v>127</v>
@@ -4720,7 +4726,7 @@
         <v>81</v>
       </c>
       <c r="AC18" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="AD18" s="39" t="s">
         <v>82</v>
@@ -4741,12 +4747,12 @@
         <v>0</v>
       </c>
       <c r="AJ18" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" ht="14.25" spans="1:36">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -4785,7 +4791,7 @@
         <v>2</v>
       </c>
       <c r="O19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -4794,19 +4800,19 @@
         <v>20</v>
       </c>
       <c r="R19" s="25" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="S19" s="25" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="T19" s="29" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="U19" s="29" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="V19" s="29" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="W19">
         <v>2</v>
@@ -4827,7 +4833,7 @@
         <v>81</v>
       </c>
       <c r="AC19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AD19" s="39" t="s">
         <v>82</v>
@@ -4848,12 +4854,12 @@
         <v>0</v>
       </c>
       <c r="AJ19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" ht="14.25" spans="1:36">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -4892,7 +4898,7 @@
         <v>2</v>
       </c>
       <c r="O20" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="P20">
         <v>0</v>
@@ -4901,19 +4907,19 @@
         <v>20</v>
       </c>
       <c r="R20" s="25" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="S20" s="25" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="T20" s="29" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="U20" s="29" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="V20" s="29" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="W20">
         <v>2</v>
@@ -4934,7 +4940,7 @@
         <v>81</v>
       </c>
       <c r="AC20" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AD20" s="39" t="s">
         <v>82</v>
@@ -4955,12 +4961,12 @@
         <v>0</v>
       </c>
       <c r="AJ20" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" ht="14.25" spans="1:36">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -4999,7 +5005,7 @@
         <v>2</v>
       </c>
       <c r="O21" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="P21">
         <v>0</v>
@@ -5008,19 +5014,19 @@
         <v>20</v>
       </c>
       <c r="R21" s="25" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="S21" s="25" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="T21" s="29" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="U21" s="29" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="V21" s="29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="W21">
         <v>2</v>
@@ -5041,7 +5047,7 @@
         <v>81</v>
       </c>
       <c r="AC21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AD21" s="39" t="s">
         <v>82</v>
@@ -5062,12 +5068,12 @@
         <v>0</v>
       </c>
       <c r="AJ21" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" ht="14.25" spans="1:36">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -5106,7 +5112,7 @@
         <v>2</v>
       </c>
       <c r="O22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="P22">
         <v>0</v>
@@ -5115,19 +5121,19 @@
         <v>20</v>
       </c>
       <c r="R22" s="25" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="S22" s="25" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="T22" s="29" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="U22" s="29" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="V22" s="29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="W22">
         <v>2</v>
@@ -5148,7 +5154,7 @@
         <v>81</v>
       </c>
       <c r="AC22" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AD22" s="39" t="s">
         <v>82</v>
@@ -5169,12 +5175,12 @@
         <v>0</v>
       </c>
       <c r="AJ22" s="46" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" s="14" customFormat="1" ht="14.25" spans="1:36">
       <c r="A23" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C23" s="14">
         <v>0</v>
@@ -5213,7 +5219,7 @@
         <v>2</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="P23" s="14">
         <v>0</v>
@@ -5222,19 +5228,19 @@
         <v>20</v>
       </c>
       <c r="R23" s="30" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="S23" s="30" t="s">
         <v>77</v>
       </c>
       <c r="T23" s="31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="U23" s="31" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="V23" s="31" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="W23" s="14">
         <v>2</v>
@@ -5255,10 +5261,10 @@
         <v>81</v>
       </c>
       <c r="AC23" s="40" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="AD23" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AE23" s="14">
         <v>0</v>
@@ -5276,12 +5282,12 @@
         <v>1</v>
       </c>
       <c r="AJ23" s="20" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" s="15" customFormat="1" ht="14.25" spans="1:36">
       <c r="A24" s="20" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C24" s="15">
         <v>0</v>
@@ -5320,7 +5326,7 @@
         <v>2</v>
       </c>
       <c r="O24" s="15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="P24" s="15">
         <v>1</v>
@@ -5329,19 +5335,19 @@
         <v>20</v>
       </c>
       <c r="R24" s="30" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="S24" s="30" t="s">
         <v>86</v>
       </c>
       <c r="T24" s="15" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="U24" s="15" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="V24" s="15" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="W24" s="15">
         <v>2</v>
@@ -5356,16 +5362,16 @@
         <v>0</v>
       </c>
       <c r="AA24" s="15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AB24" s="41" t="s">
         <v>81</v>
       </c>
       <c r="AC24" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AD24" s="15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AE24" s="15">
         <v>0</v>
@@ -5383,12 +5389,12 @@
         <v>1</v>
       </c>
       <c r="AJ24" s="20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" s="15" customFormat="1" ht="14.25" spans="1:36">
       <c r="A25" s="20" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C25" s="15">
         <v>0</v>
@@ -5427,7 +5433,7 @@
         <v>2</v>
       </c>
       <c r="O25" s="15" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="P25" s="15">
         <v>0</v>
@@ -5436,19 +5442,19 @@
         <v>20</v>
       </c>
       <c r="R25" s="30" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="S25" s="30" t="s">
         <v>94</v>
       </c>
       <c r="T25" s="15" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="U25" s="15" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="V25" s="15" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="W25" s="15">
         <v>2</v>
@@ -5463,16 +5469,16 @@
         <v>0</v>
       </c>
       <c r="AA25" s="15" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AB25" s="41" t="s">
         <v>81</v>
       </c>
       <c r="AC25" s="42" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AD25" s="15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AE25" s="15">
         <v>0</v>
@@ -5490,12 +5496,12 @@
         <v>1</v>
       </c>
       <c r="AJ25" s="20" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" s="15" customFormat="1" spans="1:36">
       <c r="A26" s="20" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C26" s="15">
         <v>0</v>
@@ -5534,7 +5540,7 @@
         <v>2</v>
       </c>
       <c r="O26" s="15" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="P26" s="15">
         <v>0</v>
@@ -5543,19 +5549,19 @@
         <v>20</v>
       </c>
       <c r="R26" s="30" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="S26" s="30" t="s">
         <v>102</v>
       </c>
       <c r="T26" s="15" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="U26" s="15" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="V26" s="15" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="W26" s="15">
         <v>2</v>
@@ -5570,16 +5576,16 @@
         <v>0</v>
       </c>
       <c r="AA26" s="15" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AB26" s="41" t="s">
         <v>81</v>
       </c>
       <c r="AC26" s="42" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AD26" s="15" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AE26" s="15">
         <v>0</v>
@@ -5597,12 +5603,12 @@
         <v>1</v>
       </c>
       <c r="AJ26" s="47" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" s="16" customFormat="1" spans="1:36">
       <c r="A27" s="21" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C27" s="16">
         <v>0</v>
@@ -5641,7 +5647,7 @@
         <v>2</v>
       </c>
       <c r="O27" s="16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="P27" s="16">
         <v>0</v>
@@ -5650,7 +5656,7 @@
         <v>20</v>
       </c>
       <c r="R27" s="33" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="S27" s="33" t="s">
         <v>77</v>
@@ -5668,13 +5674,13 @@
         <v>0</v>
       </c>
       <c r="AA27" s="16" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AB27" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC27" s="16" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AD27" s="43" t="s">
         <v>82</v>
@@ -5695,12 +5701,12 @@
         <v>2</v>
       </c>
       <c r="AJ27" s="22" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" s="17" customFormat="1" spans="1:36">
       <c r="A28" s="22" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C28" s="17">
         <v>0</v>
@@ -5739,7 +5745,7 @@
         <v>2</v>
       </c>
       <c r="O28" s="16" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P28" s="17">
         <v>0</v>
@@ -5748,7 +5754,7 @@
         <v>20</v>
       </c>
       <c r="R28" s="33" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="S28" s="33" t="s">
         <v>77</v>
@@ -5766,13 +5772,13 @@
         <v>0</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AB28" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC28" s="17" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AD28" s="44" t="s">
         <v>82</v>
@@ -5793,12 +5799,12 @@
         <v>2</v>
       </c>
       <c r="AJ28" s="22" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" s="17" customFormat="1" spans="1:36">
       <c r="A29" s="22" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C29" s="17">
         <v>0</v>
@@ -5837,7 +5843,7 @@
         <v>2</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="P29" s="17">
         <v>0</v>
@@ -5846,7 +5852,7 @@
         <v>20</v>
       </c>
       <c r="R29" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="S29" s="33" t="s">
         <v>77</v>
@@ -5864,13 +5870,13 @@
         <v>0</v>
       </c>
       <c r="AA29" s="17" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AB29" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC29" s="17" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="AD29" s="44" t="s">
         <v>82</v>
@@ -5891,12 +5897,12 @@
         <v>2</v>
       </c>
       <c r="AJ29" s="22" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" s="17" customFormat="1" spans="1:36">
       <c r="A30" s="22" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C30" s="17">
         <v>0</v>
@@ -5935,7 +5941,7 @@
         <v>2</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="P30" s="17">
         <v>0</v>
@@ -5944,7 +5950,7 @@
         <v>20</v>
       </c>
       <c r="R30" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="S30" s="33" t="s">
         <v>77</v>
@@ -5962,13 +5968,13 @@
         <v>0</v>
       </c>
       <c r="AA30" s="17" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AB30" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC30" s="17" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AD30" s="44" t="s">
         <v>82</v>
@@ -5989,12 +5995,12 @@
         <v>2</v>
       </c>
       <c r="AJ30" s="22" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" s="17" customFormat="1" spans="1:36">
       <c r="A31" s="22" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C31" s="17">
         <v>0</v>
@@ -6033,7 +6039,7 @@
         <v>2</v>
       </c>
       <c r="O31" s="17" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="P31" s="17">
         <v>0</v>
@@ -6042,7 +6048,7 @@
         <v>20</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="S31" s="33" t="s">
         <v>77</v>
@@ -6060,13 +6066,13 @@
         <v>0</v>
       </c>
       <c r="AA31" s="17" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AB31" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC31" s="17" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AD31" s="44" t="s">
         <v>82</v>
@@ -6087,12 +6093,12 @@
         <v>2</v>
       </c>
       <c r="AJ31" s="22" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" s="17" customFormat="1" spans="1:36">
       <c r="A32" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C32" s="17">
         <v>0</v>
@@ -6131,7 +6137,7 @@
         <v>2</v>
       </c>
       <c r="O32" s="17" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="P32" s="17">
         <v>0</v>
@@ -6140,7 +6146,7 @@
         <v>20</v>
       </c>
       <c r="R32" s="17" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S32" s="33" t="s">
         <v>77</v>
@@ -6158,13 +6164,13 @@
         <v>0</v>
       </c>
       <c r="AA32" s="17" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AB32" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC32" s="17" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AD32" s="44" t="s">
         <v>82</v>
@@ -6185,12 +6191,12 @@
         <v>2</v>
       </c>
       <c r="AJ32" s="22" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" s="17" customFormat="1" spans="1:36">
       <c r="A33" s="22" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C33" s="17">
         <v>0</v>
@@ -6229,7 +6235,7 @@
         <v>2</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="P33" s="17">
         <v>0</v>
@@ -6238,7 +6244,7 @@
         <v>20</v>
       </c>
       <c r="R33" s="17" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="S33" s="33" t="s">
         <v>77</v>
@@ -6256,13 +6262,13 @@
         <v>0</v>
       </c>
       <c r="AA33" s="17" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AB33" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC33" s="17" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AD33" s="44" t="s">
         <v>82</v>
@@ -6283,12 +6289,12 @@
         <v>2</v>
       </c>
       <c r="AJ33" s="22" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" s="17" customFormat="1" spans="1:36">
       <c r="A34" s="22" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C34" s="17">
         <v>0</v>
@@ -6327,7 +6333,7 @@
         <v>2</v>
       </c>
       <c r="O34" s="17" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="P34" s="17">
         <v>0</v>
@@ -6354,13 +6360,13 @@
         <v>0</v>
       </c>
       <c r="AA34" s="17" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AB34" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC34" s="17" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AD34" s="44" t="s">
         <v>82</v>
@@ -6381,12 +6387,12 @@
         <v>2</v>
       </c>
       <c r="AJ34" s="22" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" s="17" customFormat="1" spans="1:36">
       <c r="A35" s="22" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C35" s="17">
         <v>0</v>
@@ -6425,7 +6431,7 @@
         <v>2</v>
       </c>
       <c r="O35" s="17" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="P35" s="17">
         <v>0</v>
@@ -6452,13 +6458,13 @@
         <v>0</v>
       </c>
       <c r="AA35" s="17" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AB35" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC35" s="17" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AD35" s="44" t="s">
         <v>82</v>
@@ -6479,12 +6485,12 @@
         <v>2</v>
       </c>
       <c r="AJ35" s="22" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" s="17" customFormat="1" spans="1:36">
       <c r="A36" s="22" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C36" s="17">
         <v>0</v>
@@ -6523,7 +6529,7 @@
         <v>3</v>
       </c>
       <c r="O36" s="17" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="P36" s="17">
         <v>0</v>
@@ -6550,13 +6556,13 @@
         <v>0</v>
       </c>
       <c r="AA36" s="17" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AB36" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC36" s="17" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="AD36" s="44" t="s">
         <v>82</v>
@@ -6577,12 +6583,12 @@
         <v>2</v>
       </c>
       <c r="AJ36" s="22" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" s="17" customFormat="1" spans="1:36">
       <c r="A37" s="22" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C37" s="17">
         <v>0</v>
@@ -6621,7 +6627,7 @@
         <v>3</v>
       </c>
       <c r="O37" s="17" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="P37" s="17">
         <v>0</v>
@@ -6648,13 +6654,13 @@
         <v>0</v>
       </c>
       <c r="AA37" s="17" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AB37" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC37" s="17" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AD37" s="44" t="s">
         <v>82</v>
@@ -6675,12 +6681,12 @@
         <v>2</v>
       </c>
       <c r="AJ37" s="22" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" s="17" customFormat="1" spans="1:36">
       <c r="A38" s="22" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C38" s="17">
         <v>0</v>
@@ -6719,7 +6725,7 @@
         <v>3</v>
       </c>
       <c r="O38" s="17" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="P38" s="17">
         <v>0</v>
@@ -6746,13 +6752,13 @@
         <v>0</v>
       </c>
       <c r="AA38" s="17" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AB38" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC38" s="17" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="AD38" s="44" t="s">
         <v>82</v>
@@ -6773,12 +6779,12 @@
         <v>2</v>
       </c>
       <c r="AJ38" s="22" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" s="17" customFormat="1" spans="1:36">
       <c r="A39" s="22" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C39" s="17">
         <v>0</v>
@@ -6817,7 +6823,7 @@
         <v>1</v>
       </c>
       <c r="O39" s="17" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="P39" s="17">
         <v>0</v>
@@ -6844,13 +6850,13 @@
         <v>0</v>
       </c>
       <c r="AA39" s="17" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AB39" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC39" s="17" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AD39" s="44" t="s">
         <v>82</v>
@@ -6871,12 +6877,12 @@
         <v>2</v>
       </c>
       <c r="AJ39" s="22" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" s="17" customFormat="1" spans="1:36">
       <c r="A40" s="22" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C40" s="17">
         <v>0</v>
@@ -6915,7 +6921,7 @@
         <v>1</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="P40" s="17">
         <v>0</v>
@@ -6942,13 +6948,13 @@
         <v>0</v>
       </c>
       <c r="AA40" s="17" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AB40" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC40" s="17" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AD40" s="44" t="s">
         <v>82</v>
@@ -6969,12 +6975,12 @@
         <v>2</v>
       </c>
       <c r="AJ40" s="22" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" s="17" customFormat="1" spans="1:36">
       <c r="A41" s="22" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C41" s="17">
         <v>0</v>
@@ -7013,7 +7019,7 @@
         <v>1</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="P41" s="17">
         <v>0</v>
@@ -7022,7 +7028,7 @@
         <v>20</v>
       </c>
       <c r="R41" s="33" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="S41" s="33" t="s">
         <v>77</v>
@@ -7040,13 +7046,13 @@
         <v>0</v>
       </c>
       <c r="AA41" s="17" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AB41" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC41" s="17" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="AD41" s="44" t="s">
         <v>82</v>
@@ -7067,12 +7073,12 @@
         <v>2</v>
       </c>
       <c r="AJ41" s="22" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" s="17" customFormat="1" spans="1:36">
       <c r="A42" s="22" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C42" s="17">
         <v>0</v>
@@ -7111,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="O42" s="17" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="P42" s="17">
         <v>0</v>
@@ -7120,7 +7126,7 @@
         <v>20</v>
       </c>
       <c r="R42" s="33" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="S42" s="33" t="s">
         <v>77</v>
@@ -7138,13 +7144,13 @@
         <v>0</v>
       </c>
       <c r="AA42" s="17" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AB42" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC42" s="17" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AD42" s="44" t="s">
         <v>82</v>
@@ -7165,12 +7171,12 @@
         <v>2</v>
       </c>
       <c r="AJ42" s="22" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43" s="17" customFormat="1" spans="1:36">
       <c r="A43" s="22" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C43" s="17">
         <v>0</v>
@@ -7209,7 +7215,7 @@
         <v>2</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="P43" s="17">
         <v>0</v>
@@ -7218,7 +7224,7 @@
         <v>20</v>
       </c>
       <c r="R43" s="33" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="S43" s="33" t="s">
         <v>77</v>
@@ -7236,13 +7242,13 @@
         <v>0</v>
       </c>
       <c r="AA43" s="17" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AB43" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC43" s="17" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AD43" s="44" t="s">
         <v>82</v>
@@ -7263,12 +7269,12 @@
         <v>2</v>
       </c>
       <c r="AJ43" s="22" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" s="17" customFormat="1" spans="1:36">
       <c r="A44" s="22" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C44" s="17">
         <v>0</v>
@@ -7307,7 +7313,7 @@
         <v>2</v>
       </c>
       <c r="O44" s="17" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="P44" s="17">
         <v>0</v>
@@ -7316,7 +7322,7 @@
         <v>20</v>
       </c>
       <c r="R44" s="33" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="S44" s="33" t="s">
         <v>77</v>
@@ -7334,13 +7340,13 @@
         <v>0</v>
       </c>
       <c r="AA44" s="17" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AB44" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC44" s="17" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="AD44" s="44" t="s">
         <v>82</v>
@@ -7361,12 +7367,12 @@
         <v>2</v>
       </c>
       <c r="AJ44" s="22" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="45" s="17" customFormat="1" spans="1:36">
       <c r="A45" s="22" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C45" s="17">
         <v>0</v>
@@ -7405,7 +7411,7 @@
         <v>2</v>
       </c>
       <c r="O45" s="17" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="P45" s="17">
         <v>0</v>
@@ -7414,7 +7420,7 @@
         <v>20</v>
       </c>
       <c r="R45" s="33" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="S45" s="33" t="s">
         <v>77</v>
@@ -7432,13 +7438,13 @@
         <v>0</v>
       </c>
       <c r="AA45" s="17" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AB45" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC45" s="17" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AD45" s="44" t="s">
         <v>82</v>
@@ -7459,12 +7465,12 @@
         <v>2</v>
       </c>
       <c r="AJ45" s="22" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="46" s="17" customFormat="1" spans="1:36">
       <c r="A46" s="22" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C46" s="17">
         <v>0</v>
@@ -7503,7 +7509,7 @@
         <v>2</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="P46" s="17">
         <v>0</v>
@@ -7512,7 +7518,7 @@
         <v>20</v>
       </c>
       <c r="R46" s="33" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="S46" s="33" t="s">
         <v>77</v>
@@ -7530,13 +7536,13 @@
         <v>0</v>
       </c>
       <c r="AA46" s="17" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AB46" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC46" s="17" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AD46" s="44" t="s">
         <v>82</v>
@@ -7557,12 +7563,12 @@
         <v>2</v>
       </c>
       <c r="AJ46" s="22" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47" s="17" customFormat="1" spans="1:36">
       <c r="A47" s="22" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C47" s="17">
         <v>0</v>
@@ -7601,7 +7607,7 @@
         <v>2</v>
       </c>
       <c r="O47" s="17" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="P47" s="17">
         <v>0</v>
@@ -7610,7 +7616,7 @@
         <v>20</v>
       </c>
       <c r="R47" s="33" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="S47" s="33" t="s">
         <v>77</v>
@@ -7628,13 +7634,13 @@
         <v>0</v>
       </c>
       <c r="AA47" s="17" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AB47" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC47" s="17" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="AD47" s="44" t="s">
         <v>82</v>
@@ -7655,12 +7661,12 @@
         <v>2</v>
       </c>
       <c r="AJ47" s="22" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="48" s="17" customFormat="1" spans="1:36">
       <c r="A48" s="22" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C48" s="17">
         <v>0</v>
@@ -7699,7 +7705,7 @@
         <v>3</v>
       </c>
       <c r="O48" s="17" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="P48" s="17">
         <v>0</v>
@@ -7708,7 +7714,7 @@
         <v>20</v>
       </c>
       <c r="R48" s="33" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="S48" s="33" t="s">
         <v>77</v>
@@ -7726,13 +7732,13 @@
         <v>0</v>
       </c>
       <c r="AA48" s="17" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="AB48" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC48" s="17" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AD48" s="44" t="s">
         <v>82</v>
@@ -7753,12 +7759,12 @@
         <v>2</v>
       </c>
       <c r="AJ48" s="22" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="49" s="17" customFormat="1" spans="1:36">
       <c r="A49" s="22" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C49" s="17">
         <v>0</v>
@@ -7797,7 +7803,7 @@
         <v>3</v>
       </c>
       <c r="O49" s="17" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="P49" s="17">
         <v>0</v>
@@ -7806,7 +7812,7 @@
         <v>20</v>
       </c>
       <c r="R49" s="33" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="S49" s="33" t="s">
         <v>77</v>
@@ -7824,13 +7830,13 @@
         <v>0</v>
       </c>
       <c r="AA49" s="17" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AB49" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC49" s="17" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AD49" s="44" t="s">
         <v>82</v>
@@ -7851,12 +7857,12 @@
         <v>2</v>
       </c>
       <c r="AJ49" s="22" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" s="17" customFormat="1" spans="1:36">
       <c r="A50" s="22" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C50" s="17">
         <v>0</v>
@@ -7895,7 +7901,7 @@
         <v>3</v>
       </c>
       <c r="O50" s="17" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="P50" s="17">
         <v>0</v>
@@ -7904,7 +7910,7 @@
         <v>20</v>
       </c>
       <c r="R50" s="33" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="S50" s="33" t="s">
         <v>77</v>
@@ -7922,13 +7928,13 @@
         <v>0</v>
       </c>
       <c r="AA50" s="17" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AB50" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC50" s="17" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AD50" s="44" t="s">
         <v>82</v>
@@ -7949,12 +7955,12 @@
         <v>2</v>
       </c>
       <c r="AJ50" s="22" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" s="17" customFormat="1" spans="1:36">
       <c r="A51" s="22" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C51" s="17">
         <v>0</v>
@@ -7993,7 +7999,7 @@
         <v>2</v>
       </c>
       <c r="O51" s="17" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="P51" s="17">
         <v>0</v>
@@ -8002,7 +8008,7 @@
         <v>20</v>
       </c>
       <c r="R51" s="33" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="S51" s="33" t="s">
         <v>77</v>
@@ -8020,13 +8026,13 @@
         <v>0</v>
       </c>
       <c r="AA51" s="17" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AB51" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC51" s="17" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="AD51" s="44" t="s">
         <v>82</v>
@@ -8047,12 +8053,12 @@
         <v>2</v>
       </c>
       <c r="AJ51" s="22" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="52" s="17" customFormat="1" spans="1:36">
       <c r="A52" s="22" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C52" s="17">
         <v>0</v>
@@ -8091,7 +8097,7 @@
         <v>2</v>
       </c>
       <c r="O52" s="17" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="P52" s="17">
         <v>0</v>
@@ -8100,7 +8106,7 @@
         <v>20</v>
       </c>
       <c r="R52" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="S52" s="33" t="s">
         <v>77</v>
@@ -8118,13 +8124,13 @@
         <v>0</v>
       </c>
       <c r="AA52" s="17" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AB52" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC52" s="17" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AD52" s="44" t="s">
         <v>82</v>
@@ -8145,12 +8151,12 @@
         <v>2</v>
       </c>
       <c r="AJ52" s="22" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53" s="17" customFormat="1" spans="1:36">
       <c r="A53" s="22" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C53" s="17">
         <v>0</v>
@@ -8189,7 +8195,7 @@
         <v>2</v>
       </c>
       <c r="O53" s="17" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="P53" s="17">
         <v>0</v>
@@ -8198,7 +8204,7 @@
         <v>20</v>
       </c>
       <c r="R53" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="S53" s="33" t="s">
         <v>77</v>
@@ -8216,13 +8222,13 @@
         <v>0</v>
       </c>
       <c r="AA53" s="17" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="AB53" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC53" s="17" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="AD53" s="44" t="s">
         <v>82</v>
@@ -8243,12 +8249,12 @@
         <v>2</v>
       </c>
       <c r="AJ53" s="22" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="54" s="17" customFormat="1" spans="1:36">
       <c r="A54" s="22" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C54" s="17">
         <v>0</v>
@@ -8287,7 +8293,7 @@
         <v>3</v>
       </c>
       <c r="O54" s="17" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="P54" s="17">
         <v>0</v>
@@ -8296,7 +8302,7 @@
         <v>20</v>
       </c>
       <c r="R54" s="17" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="S54" s="33" t="s">
         <v>77</v>
@@ -8314,13 +8320,13 @@
         <v>0</v>
       </c>
       <c r="AA54" s="17" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AB54" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC54" s="17" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="AD54" s="44" t="s">
         <v>82</v>
@@ -8341,12 +8347,12 @@
         <v>2</v>
       </c>
       <c r="AJ54" s="22" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="55" s="17" customFormat="1" spans="1:36">
       <c r="A55" s="22" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C55" s="17">
         <v>0</v>
@@ -8385,7 +8391,7 @@
         <v>3</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="P55" s="17">
         <v>0</v>
@@ -8394,7 +8400,7 @@
         <v>20</v>
       </c>
       <c r="R55" s="17" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S55" s="33" t="s">
         <v>77</v>
@@ -8412,13 +8418,13 @@
         <v>0</v>
       </c>
       <c r="AA55" s="17" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="AB55" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC55" s="17" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AD55" s="44" t="s">
         <v>82</v>
@@ -8439,12 +8445,12 @@
         <v>2</v>
       </c>
       <c r="AJ55" s="22" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="56" s="17" customFormat="1" spans="1:36">
       <c r="A56" s="22" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C56" s="17">
         <v>0</v>
@@ -8483,7 +8489,7 @@
         <v>3</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="P56" s="17">
         <v>0</v>
@@ -8492,7 +8498,7 @@
         <v>20</v>
       </c>
       <c r="R56" s="17" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="S56" s="33" t="s">
         <v>77</v>
@@ -8510,13 +8516,13 @@
         <v>0</v>
       </c>
       <c r="AA56" s="17" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="AB56" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC56" s="17" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="AD56" s="44" t="s">
         <v>82</v>
@@ -8537,12 +8543,12 @@
         <v>2</v>
       </c>
       <c r="AJ56" s="22" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57" s="17" customFormat="1" spans="1:36">
       <c r="A57" s="22" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C57" s="17">
         <v>0</v>
@@ -8581,7 +8587,7 @@
         <v>2</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="P57" s="17">
         <v>0</v>
@@ -8590,7 +8596,7 @@
         <v>20</v>
       </c>
       <c r="R57" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="S57" s="33" t="s">
         <v>77</v>
@@ -8608,13 +8614,13 @@
         <v>0</v>
       </c>
       <c r="AA57" s="17" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="AB57" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC57" s="17" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="AD57" s="44" t="s">
         <v>82</v>
@@ -8635,12 +8641,12 @@
         <v>2</v>
       </c>
       <c r="AJ57" s="22" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" s="17" customFormat="1" ht="14.25" spans="1:36">
       <c r="A58" s="22" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C58" s="17">
         <v>0</v>
@@ -8679,7 +8685,7 @@
         <v>2</v>
       </c>
       <c r="O58" s="17" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="P58" s="17">
         <v>0</v>
@@ -8688,7 +8694,7 @@
         <v>20</v>
       </c>
       <c r="R58" s="17" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="S58" s="33" t="s">
         <v>77</v>
@@ -8706,13 +8712,13 @@
         <v>0</v>
       </c>
       <c r="AA58" s="17" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="AB58" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC58" s="17" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AD58" s="44" t="s">
         <v>82</v>
@@ -8733,12 +8739,12 @@
         <v>2</v>
       </c>
       <c r="AJ58" s="23" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" s="18" customFormat="1" ht="14.25" spans="1:36">
       <c r="A59" s="23" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C59" s="18">
         <v>0</v>
@@ -8777,7 +8783,7 @@
         <v>2</v>
       </c>
       <c r="O59" s="17" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="P59" s="18">
         <v>0</v>
@@ -8786,7 +8792,7 @@
         <v>20</v>
       </c>
       <c r="R59" s="17" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S59" s="33" t="s">
         <v>77</v>
@@ -8804,13 +8810,13 @@
         <v>0</v>
       </c>
       <c r="AA59" s="18" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AB59" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC59" s="18" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="AD59" s="45" t="s">
         <v>82</v>
@@ -8831,12 +8837,12 @@
         <v>2</v>
       </c>
       <c r="AJ59" s="22" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="60" s="17" customFormat="1" spans="1:36">
       <c r="A60" s="22" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C60" s="17">
         <v>0</v>
@@ -8875,7 +8881,7 @@
         <v>2</v>
       </c>
       <c r="O60" s="17" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="P60" s="17">
         <v>0</v>
@@ -8884,7 +8890,7 @@
         <v>20</v>
       </c>
       <c r="R60" s="17" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="S60" s="33" t="s">
         <v>77</v>
@@ -8902,13 +8908,13 @@
         <v>0</v>
       </c>
       <c r="AA60" s="17" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="AB60" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC60" s="17" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="AD60" s="44" t="s">
         <v>82</v>
@@ -8929,12 +8935,12 @@
         <v>2</v>
       </c>
       <c r="AJ60" s="22" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="61" s="17" customFormat="1" ht="14.25" spans="1:36">
       <c r="A61" s="22" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C61" s="17">
         <v>0</v>
@@ -8973,7 +8979,7 @@
         <v>2</v>
       </c>
       <c r="O61" s="17" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="P61" s="17">
         <v>0</v>
@@ -8982,7 +8988,7 @@
         <v>20</v>
       </c>
       <c r="R61" s="17" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S61" s="33" t="s">
         <v>77</v>
@@ -9000,13 +9006,13 @@
         <v>0</v>
       </c>
       <c r="AA61" s="17" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AB61" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC61" s="17" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="AD61" s="44" t="s">
         <v>82</v>
@@ -9027,12 +9033,12 @@
         <v>2</v>
       </c>
       <c r="AJ61" s="23" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="62" s="18" customFormat="1" ht="14.25" spans="1:36">
       <c r="A62" s="23" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C62" s="18">
         <v>0</v>
@@ -9071,7 +9077,7 @@
         <v>2</v>
       </c>
       <c r="O62" s="17" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="P62" s="18">
         <v>0</v>
@@ -9080,7 +9086,7 @@
         <v>20</v>
       </c>
       <c r="R62" s="17" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="S62" s="33" t="s">
         <v>77</v>
@@ -9098,13 +9104,13 @@
         <v>0</v>
       </c>
       <c r="AA62" s="18" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="AB62" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AC62" s="18" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="AD62" s="45" t="s">
         <v>82</v>
@@ -9125,7 +9131,7 @@
         <v>2</v>
       </c>
       <c r="AJ62" s="18" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -9146,7 +9152,7 @@
   <sheetPr/>
   <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AA3" sqref="AA3:AF3"/>
     </sheetView>
   </sheetViews>
@@ -9160,97 +9166,97 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="AE1" s="5" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="AF1" s="5" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" spans="1:32">
@@ -10042,13 +10048,13 @@
         <v>47</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>51</v>
@@ -10060,73 +10066,73 @@
         <v>52</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="V10" s="8" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="W10" s="8" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="X10" s="8" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="Y10" s="8" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="Z10" s="8" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="AA10" s="8" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="AB10" s="8" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="AC10" s="8" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AD10" s="8" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AE10" s="8" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="AF10" s="8" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:1">
@@ -10218,12 +10224,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B2" s="3">
         <v>8</v>
@@ -10231,7 +10237,7 @@
     </row>
     <row r="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -10295,10 +10301,10 @@
     </row>
     <row r="11" customFormat="1" spans="1:2">
       <c r="A11" s="4" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:2">

</xml_diff>

<commit_message>
Chat channel && chat type Skill & icon
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/NPC.xlsx
+++ b/_Out/NFDataCfg/Excel/NPC.xlsx
@@ -2030,10 +2030,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -2076,6 +2076,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2084,15 +2092,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2100,14 +2100,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2129,14 +2129,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -2144,18 +2136,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2174,8 +2175,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2188,9 +2212,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2199,29 +2222,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2302,7 +2302,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2314,7 +2314,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2326,157 +2470,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2675,15 +2675,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2695,6 +2686,50 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2717,19 +2752,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2748,177 +2772,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3490,10 +3490,10 @@
   <sheetPr/>
   <dimension ref="A1:AO39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="U11" sqref="U11:W20"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -8183,9 +8183,7 @@
     <col min="16" max="16" width="14.6634615384615" customWidth="1"/>
     <col min="17" max="17" width="13.6634615384615" customWidth="1"/>
     <col min="18" max="19" width="23" customWidth="1"/>
-    <col min="20" max="20" width="27" customWidth="1"/>
-    <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="23" width="27" customWidth="1"/>
+    <col min="20" max="23" width="27" customWidth="1"/>
     <col min="25" max="25" width="17.1634615384615" customWidth="1"/>
     <col min="26" max="26" width="13.8365384615385" customWidth="1"/>
     <col min="27" max="27" width="20" customWidth="1"/>
@@ -9709,7 +9707,6 @@
       <c r="T13" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U13" s="15"/>
       <c r="X13" s="14">
         <v>4</v>
       </c>
@@ -9927,7 +9924,6 @@
       <c r="T15" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U15" s="15"/>
       <c r="X15" s="14">
         <v>4</v>
       </c>
@@ -10145,7 +10141,6 @@
       <c r="T17" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U17" s="15"/>
       <c r="X17" s="14">
         <v>4</v>
       </c>
@@ -10363,7 +10358,6 @@
       <c r="T19" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U19" s="15"/>
       <c r="X19" s="14">
         <v>4</v>
       </c>
@@ -10581,7 +10575,6 @@
       <c r="T21" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U21" s="15"/>
       <c r="X21" s="14">
         <v>4</v>
       </c>
@@ -10799,7 +10792,6 @@
       <c r="T23" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U23" s="15"/>
       <c r="X23" s="14">
         <v>4</v>
       </c>
@@ -11017,7 +11009,6 @@
       <c r="T25" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U25" s="15"/>
       <c r="X25" s="14">
         <v>4</v>
       </c>
@@ -11235,7 +11226,6 @@
       <c r="T27" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U27" s="15"/>
       <c r="X27" s="14">
         <v>4</v>
       </c>
@@ -11453,7 +11443,6 @@
       <c r="T29" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U29" s="15"/>
       <c r="X29" s="14">
         <v>4</v>
       </c>
@@ -11671,7 +11660,6 @@
       <c r="T31" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U31" s="15"/>
       <c r="X31" s="14">
         <v>4</v>
       </c>
@@ -11889,7 +11877,6 @@
       <c r="T33" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U33" s="15"/>
       <c r="X33" s="14">
         <v>4</v>
       </c>
@@ -12107,7 +12094,6 @@
       <c r="T35" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U35" s="15"/>
       <c r="X35" s="14">
         <v>4</v>
       </c>
@@ -12325,7 +12311,6 @@
       <c r="T37" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U37" s="15"/>
       <c r="X37" s="14">
         <v>4</v>
       </c>
@@ -12543,7 +12528,6 @@
       <c r="T39" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U39" s="15"/>
       <c r="X39" s="14">
         <v>4</v>
       </c>
@@ -12761,7 +12745,6 @@
       <c r="T41" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U41" s="15"/>
       <c r="X41" s="14">
         <v>4</v>
       </c>
@@ -12979,7 +12962,6 @@
       <c r="T43" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U43" s="16"/>
       <c r="X43" s="14">
         <v>4</v>
       </c>
@@ -13197,7 +13179,6 @@
       <c r="T45" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="U45" s="15"/>
       <c r="X45" s="14">
         <v>4</v>
       </c>
@@ -13307,7 +13288,6 @@
       <c r="T46" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="U46" s="16"/>
       <c r="X46" s="15">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
element module && class module for multi-thread feature
now we can use element module and class module when using component by async mode.
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/NPC.xlsx
+++ b/_Out/NFDataCfg/Excel/NPC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21440" activeTab="1"/>
+    <workbookView windowHeight="23360"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127">
   <si>
     <t>Id</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Prefab</t>
   </si>
   <si>
-    <t>Climb</t>
+    <t>CommonCD</t>
   </si>
   <si>
     <t>DropPackList</t>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>客户端预设模型</t>
-  </si>
-  <si>
-    <t>Move类型</t>
   </si>
   <si>
     <t>掉落列表</t>
@@ -409,10 +406,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -455,33 +452,11 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -492,9 +467,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,36 +477,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -546,7 +506,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -562,14 +567,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -577,9 +575,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -592,21 +590,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -651,7 +648,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,7 +684,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,7 +738,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,37 +756,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,13 +780,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,91 +816,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,16 +967,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -996,15 +998,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1020,6 +1013,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1041,11 +1049,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1058,168 +1064,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1701,10 +1692,10 @@
   <sheetPr/>
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1855,7 +1846,7 @@
         <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>29</v>
@@ -2560,67 +2551,65 @@
       <c r="J10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="O10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="R10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R10" s="4" t="s">
+      <c r="S10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="U10" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="U10" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="V10" s="15" t="s">
         <v>20</v>
       </c>
       <c r="W10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="X10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="X10" s="4" t="s">
+      <c r="Y10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="Y10" s="4" t="s">
+      <c r="Z10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="4" t="s">
+      <c r="AA10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AA10" s="4" t="s">
+      <c r="AB10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AB10" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="AC10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" ht="17.55" spans="1:29">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2644,17 +2633,17 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="12"/>
@@ -2663,31 +2652,31 @@
         <v>2</v>
       </c>
       <c r="S11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11" s="16" t="s">
+      <c r="V11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="V11" s="17" t="s">
+      <c r="W11" t="s">
         <v>68</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="X11" s="18" t="s">
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="s">
         <v>70</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>71</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -2698,7 +2687,7 @@
     </row>
     <row r="12" ht="17.55" spans="1:29">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2722,17 +2711,17 @@
         <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N12" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="12"/>
@@ -2741,32 +2730,32 @@
         <v>2</v>
       </c>
       <c r="S12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12" s="16" t="s">
+      <c r="V12" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="V12" s="17" t="s">
+      <c r="W12" t="s">
         <v>68</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="X12" s="18" t="s">
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="s">
         <v>70</v>
       </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>71</v>
-      </c>
       <c r="AB12">
         <v>0</v>
       </c>
@@ -2774,9 +2763,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="17.55" spans="1:29">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2800,17 +2789,17 @@
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N13" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -2819,42 +2808,42 @@
         <v>2</v>
       </c>
       <c r="S13" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T13">
         <v>0</v>
       </c>
       <c r="U13" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="V13" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W13" t="s">
+        <v>72</v>
+      </c>
+      <c r="X13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="s">
         <v>77</v>
       </c>
-      <c r="V13" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W13" t="s">
-        <v>73</v>
-      </c>
-      <c r="X13" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13" t="s">
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14" t="s">
         <v>78</v>
-      </c>
-      <c r="AB13">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" ht="17.55" spans="1:29">
-      <c r="A14" t="s">
-        <v>79</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -2878,17 +2867,17 @@
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>82</v>
       </c>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
@@ -2897,42 +2886,42 @@
         <v>2</v>
       </c>
       <c r="S14" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T14">
         <v>0</v>
       </c>
       <c r="U14" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="V14" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W14" t="s">
+        <v>78</v>
+      </c>
+      <c r="X14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="s">
         <v>83</v>
       </c>
-      <c r="V14" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W14" t="s">
-        <v>79</v>
-      </c>
-      <c r="X14" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14" t="s">
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" t="s">
         <v>84</v>
-      </c>
-      <c r="AB14">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" ht="17.55" spans="1:29">
-      <c r="A15" t="s">
-        <v>85</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -2956,17 +2945,17 @@
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
@@ -2975,42 +2964,42 @@
         <v>2</v>
       </c>
       <c r="S15" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T15">
         <v>0</v>
       </c>
       <c r="U15" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="V15" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W15" t="s">
+        <v>84</v>
+      </c>
+      <c r="X15" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="s">
         <v>89</v>
       </c>
-      <c r="V15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W15" t="s">
-        <v>85</v>
-      </c>
-      <c r="X15" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15" t="s">
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" t="s">
         <v>90</v>
-      </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" ht="17.55" spans="1:29">
-      <c r="A16" t="s">
-        <v>91</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -3034,17 +3023,17 @@
         <v>2</v>
       </c>
       <c r="J16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N16" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
@@ -3053,42 +3042,42 @@
         <v>2</v>
       </c>
       <c r="S16" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T16">
         <v>0</v>
       </c>
       <c r="U16" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="V16" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W16" t="s">
+        <v>90</v>
+      </c>
+      <c r="X16" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="s">
         <v>95</v>
       </c>
-      <c r="V16" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W16" t="s">
-        <v>91</v>
-      </c>
-      <c r="X16" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="Z16">
-        <v>0</v>
-      </c>
-      <c r="AA16" t="s">
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
+      <c r="A17" t="s">
         <v>96</v>
-      </c>
-      <c r="AB16">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" ht="17.55" spans="1:29">
-      <c r="A17" t="s">
-        <v>97</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -3112,17 +3101,17 @@
         <v>2</v>
       </c>
       <c r="J17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="N17" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="N17" s="11" t="s">
-        <v>100</v>
       </c>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
@@ -3131,42 +3120,42 @@
         <v>2</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T17">
         <v>0</v>
       </c>
       <c r="U17" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="V17" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W17" t="s">
+        <v>96</v>
+      </c>
+      <c r="X17" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="s">
         <v>101</v>
       </c>
-      <c r="V17" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W17" t="s">
-        <v>97</v>
-      </c>
-      <c r="X17" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AA17" t="s">
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
+      <c r="A18" t="s">
         <v>102</v>
-      </c>
-      <c r="AB17">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" ht="17.55" spans="1:29">
-      <c r="A18" t="s">
-        <v>103</v>
       </c>
       <c r="C18">
         <v>7</v>
@@ -3190,17 +3179,17 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="N18" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="N18" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
@@ -3209,42 +3198,42 @@
         <v>2</v>
       </c>
       <c r="S18" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T18">
         <v>0</v>
       </c>
       <c r="U18" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="V18" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W18" t="s">
+        <v>102</v>
+      </c>
+      <c r="X18" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="s">
         <v>107</v>
       </c>
-      <c r="V18" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W18" t="s">
-        <v>103</v>
-      </c>
-      <c r="X18" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18" t="s">
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
+      <c r="A19" t="s">
         <v>108</v>
-      </c>
-      <c r="AB18">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" ht="17.55" spans="1:29">
-      <c r="A19" t="s">
-        <v>109</v>
       </c>
       <c r="C19">
         <v>8</v>
@@ -3268,17 +3257,17 @@
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="N19" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="N19" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
@@ -3287,42 +3276,42 @@
         <v>2</v>
       </c>
       <c r="S19" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T19">
         <v>0</v>
       </c>
       <c r="U19" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="V19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W19" t="s">
+        <v>108</v>
+      </c>
+      <c r="X19" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="s">
         <v>113</v>
       </c>
-      <c r="V19" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W19" t="s">
-        <v>109</v>
-      </c>
-      <c r="X19" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-      <c r="Z19">
-        <v>0</v>
-      </c>
-      <c r="AA19" t="s">
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
+      <c r="A20" t="s">
         <v>114</v>
-      </c>
-      <c r="AB19">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" ht="17.55" spans="1:29">
-      <c r="A20" t="s">
-        <v>115</v>
       </c>
       <c r="C20">
         <v>9</v>
@@ -3346,17 +3335,17 @@
         <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="N20" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="N20" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="O20" s="11"/>
       <c r="P20" s="11"/>
@@ -3365,31 +3354,31 @@
         <v>2</v>
       </c>
       <c r="S20" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T20">
         <v>0</v>
       </c>
       <c r="U20" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="V20" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W20" t="s">
+        <v>114</v>
+      </c>
+      <c r="X20" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="s">
         <v>119</v>
-      </c>
-      <c r="V20" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W20" t="s">
-        <v>115</v>
-      </c>
-      <c r="X20" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
-      <c r="Z20">
-        <v>0</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>120</v>
       </c>
       <c r="AB20">
         <v>0</v>
@@ -3400,7 +3389,7 @@
     </row>
     <row r="21" spans="1:29">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -3424,17 +3413,17 @@
         <v>2</v>
       </c>
       <c r="J21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="N21" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>124</v>
       </c>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
@@ -3443,31 +3432,31 @@
         <v>2</v>
       </c>
       <c r="S21" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T21">
         <v>0</v>
       </c>
       <c r="U21" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="V21" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W21" t="s">
+        <v>120</v>
+      </c>
+      <c r="X21" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="s">
         <v>125</v>
-      </c>
-      <c r="V21" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W21" t="s">
-        <v>121</v>
-      </c>
-      <c r="X21" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>126</v>
       </c>
       <c r="AB21">
         <v>0</v>
@@ -3494,7 +3483,7 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3507,7 +3496,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor for generate tool
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/NPC.xlsx
+++ b/_Out/NFDataCfg/Excel/NPC.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="32240" windowHeight="20800"/>
+    <workbookView windowHeight="21600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
     <sheet name="Include" sheetId="2" r:id="rId2"/>
+    <sheet name="Ref" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -415,10 +416,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -461,6 +462,28 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -469,31 +492,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,6 +519,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -537,8 +553,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -546,7 +569,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -567,14 +598,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -583,34 +606,12 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -657,7 +658,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,13 +712,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,37 +790,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,109 +826,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,6 +977,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -987,15 +1006,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1015,17 +1025,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1041,20 +1045,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1078,148 +1079,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1305,39 +1306,39 @@
     <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
     <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1701,7 +1702,7 @@
   <sheetPr/>
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="S12" sqref="S12"/>
@@ -2535,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" s="4" customFormat="1" ht="68.75" spans="1:29">
+    <row r="10" s="4" customFormat="1" ht="84.75" spans="1:29">
       <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
@@ -3567,22 +3568,39 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.20192307692308" defaultRowHeight="16.8"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.20192307692308" defaultRowHeight="16.8" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>